<commit_message>
Modifca periodo dei grafici per incremento, inserimento parziale dei dati del PDP
</commit_message>
<xml_diff>
--- a/DocumentazioneEsterna/PianoDiQualifica/res/ResocontoAttivitaDiVerifica/res/metriche/grafici/qualitàProcesso/graficiProcessiOrganizzativi.xlsx
+++ b/DocumentazioneEsterna/PianoDiQualifica/res/ResocontoAttivitaDiVerifica/res/metriche/grafici/qualitàProcesso/graficiProcessiOrganizzativi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Università\Terzo anno\SWE\Progetto\Documentazione\DocumentazioneEsterna\PianoDiQualifica\res\ResocontoAttivitaDiVerifica\res\metriche\grafici\qualitàProcesso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{798B8F49-8344-498F-B55B-50EF3B9BB3F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9BBC95-42CF-470F-AF2A-4CDF15EE1399}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{32F62035-8081-4F2C-A1C6-0EA80AA4F9D3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="33">
   <si>
     <t>Accettabile</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>PD</t>
-  </si>
-  <si>
-    <t>VC</t>
   </si>
   <si>
     <t>AC</t>
@@ -119,18 +116,36 @@
   <si>
     <t>BV</t>
   </si>
+  <si>
+    <t>Incremento 5</t>
+  </si>
+  <si>
+    <t>Incremento 6</t>
+  </si>
+  <si>
+    <t>Incremento 7</t>
+  </si>
+  <si>
+    <t>Incremento 8</t>
+  </si>
+  <si>
+    <t>Incremento 9</t>
+  </si>
+  <si>
+    <t>Incremento 10</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
+    <numFmt numFmtId="5" formatCode="&quot;€&quot;\ #,##0;\-&quot;€&quot;\ #,##0"/>
     <numFmt numFmtId="164" formatCode="#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]"/>
     <numFmt numFmtId="165" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
-    <numFmt numFmtId="166" formatCode="&quot;€&quot;\ #,##0"/>
     <numFmt numFmtId="167" formatCode="#,##0.00\ [$€-1];[Red]\-#,##0.00\ [$€-1]"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,6 +178,12 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -200,7 +221,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -243,20 +264,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -264,21 +272,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -290,22 +294,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="5" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -434,9 +433,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Pianificazione!$B$6:$B$10</c:f>
+              <c:f>Pianificazione!$B$6:$B$13</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>A</c:v>
                 </c:pt>
@@ -444,24 +443,54 @@
                   <c:v>PA</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>PD</c:v>
+                  <c:v>Incremento 5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>VC</c:v>
+                  <c:v>Incremento 6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Incremento 7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Incremento 8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Incremento 9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Incremento 10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Pianificazione!$D$6:$D$10</c:f>
+              <c:f>Pianificazione!$D$6:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>13154</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>13154</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13154</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13154</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13154</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13154</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13154</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>13154</c:v>
                 </c:pt>
               </c:numCache>
@@ -501,9 +530,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Pianificazione!$B$6:$B$10</c:f>
+              <c:f>Pianificazione!$B$6:$B$13</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>A</c:v>
                 </c:pt>
@@ -511,25 +540,55 @@
                   <c:v>PA</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>PD</c:v>
+                  <c:v>Incremento 5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>VC</c:v>
+                  <c:v>Incremento 6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Incremento 7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Incremento 8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Incremento 9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Incremento 10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Pianificazione!$E$6:$E$10</c:f>
+              <c:f>Pianificazione!$E$6:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4482</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1197</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1441</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1411</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>521</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>583</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -650,9 +709,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Pianificazione!$B$6:$B$10</c:f>
+              <c:f>Pianificazione!$B$6:$B$13</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>A</c:v>
                 </c:pt>
@@ -660,25 +719,55 @@
                   <c:v>PA</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>PD</c:v>
+                  <c:v>Incremento 5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>VC</c:v>
+                  <c:v>Incremento 6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Incremento 7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Incremento 8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Incremento 9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Incremento 10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Pianificazione!$C$6:$C$10</c:f>
+              <c:f>Pianificazione!$C$6:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4417</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>967</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1326</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1141</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1396</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>521</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>583</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -813,8 +902,6 @@
         <c:axId val="365909112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="20000"/>
-          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -921,7 +1008,6 @@
         <c:crossAx val="365907192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="3000"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1115,9 +1201,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Pianificazione!$B$31:$B$34</c:f>
+              <c:f>Pianificazione!$B$31:$B$38</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>A</c:v>
                 </c:pt>
@@ -1125,25 +1211,55 @@
                   <c:v>PA</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>PD</c:v>
+                  <c:v>Incremento 5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>VC</c:v>
+                  <c:v>Incremento 6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Incremento 7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Incremento 8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Incremento 9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Incremento 10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Pianificazione!$D$31:$D$34</c:f>
+              <c:f>Pianificazione!$D$31:$D$38</c:f>
               <c:numCache>
                 <c:formatCode>#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4706.1000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1057.3499999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1256.8499999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1513.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1481.55</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>547.04999999999995</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>612.15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1182,9 +1298,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Pianificazione!$B$31:$B$34</c:f>
+              <c:f>Pianificazione!$B$31:$B$38</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>A</c:v>
                 </c:pt>
@@ -1192,25 +1308,55 @@
                   <c:v>PA</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>PD</c:v>
+                  <c:v>Incremento 5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>VC</c:v>
+                  <c:v>Incremento 6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Incremento 7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Incremento 8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Incremento 9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Incremento 10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Pianificazione!$E$31:$E$34</c:f>
+              <c:f>Pianificazione!$E$31:$E$38</c:f>
               <c:numCache>
                 <c:formatCode>#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4482</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1197</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1441</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1411</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>521</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>583</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1274,6 +1420,28 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.3796237581906573E-2"/>
+                  <c:y val="-5.3367838088610529E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-E9EE-44A5-AB14-A23A3AFB8CC4}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -1303,6 +1471,7 @@
                 <a:endParaRPr lang="it-IT"/>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="t"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -1332,9 +1501,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Pianificazione!$B$31:$B$34</c:f>
+              <c:f>Pianificazione!$B$31:$B$38</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>A</c:v>
                 </c:pt>
@@ -1342,25 +1511,55 @@
                   <c:v>PA</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>PD</c:v>
+                  <c:v>Incremento 5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>VC</c:v>
+                  <c:v>Incremento 6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Incremento 7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Incremento 8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Incremento 9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Incremento 10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Pianificazione!$C$31:$C$34</c:f>
+              <c:f>Pianificazione!$C$31:$C$38</c:f>
               <c:numCache>
                 <c:formatCode>#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4417</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>967</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1326</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1141</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1396</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>521</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>583</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1495,8 +1694,6 @@
         <c:axId val="365909112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="8000"/>
-          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1603,7 +1800,6 @@
         <c:crossAx val="365907192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="1000"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1804,7 +2000,14 @@
           </c:marker>
           <c:dLbls>
             <c:dLbl>
-              <c:idx val="1"/>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.3817022475868385E-2"/>
+                  <c:y val="-8.2827360241243403E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -1814,7 +2017,29 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000001-4CC3-41F8-A162-36DF2CC34A3B}"/>
+                  <c16:uniqueId val="{00000002-9217-4D4C-AAA7-6C47124ECA0B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.4943281899527936E-2"/>
+                  <c:y val="-4.9685397819531428E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-9217-4D4C-AAA7-6C47124ECA0B}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1847,12 +2072,14 @@
                 <a:endParaRPr lang="it-IT"/>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="t"/>
             <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
+            <c:showVal val="1"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
@@ -1875,9 +2102,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Pianificazione!$B$61:$B$64</c:f>
+              <c:f>Pianificazione!$B$61:$B$68</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>A</c:v>
                 </c:pt>
@@ -1885,25 +2112,55 @@
                   <c:v>PA</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>PD</c:v>
+                  <c:v>Incremento 5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>VC</c:v>
+                  <c:v>Incremento 6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Incremento 7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Incremento 8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Incremento 9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Incremento 10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Pianificazione!$C$61:$C$64</c:f>
+              <c:f>Pianificazione!$C$61:$C$68</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0" formatCode="0%">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>6.4999999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.29E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1993,7 +2250,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -2038,7 +2295,6 @@
         <c:axId val="365909112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="3.0000000000000006E-2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2090,7 +2346,6 @@
         <c:crossAx val="365907192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="1.0000000000000002E-2"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2289,11 +2544,91 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.5585852180652433E-2"/>
+                  <c:y val="-4.9685397819531428E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-3A5C-4087-9D63-EA656B29C2DF}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Pianificazione!$B$77:$B$80</c:f>
+              <c:f>Pianificazione!$B$77:$B$84</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>A</c:v>
                 </c:pt>
@@ -2301,25 +2636,55 @@
                   <c:v>PA</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>PD</c:v>
+                  <c:v>Incremento 5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>VC</c:v>
+                  <c:v>Incremento 6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Incremento 7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Incremento 8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Incremento 9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Incremento 10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Pianificazione!$C$77:$C$80</c:f>
+              <c:f>Pianificazione!$C$77:$C$84</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:formatCode>"€"#,##0_);\("€"#,##0\)</c:formatCode>
+                <c:ptCount val="8"/>
                 <c:pt idx="0" formatCode="#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-65</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2409,7 +2774,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -2759,6 +3124,50 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.3722081307686888E-2"/>
+                  <c:y val="-7.54624797030852E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-BB51-4C4B-8E1B-307D303008E1}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.6458817727048543E-2"/>
+                  <c:y val="-4.6002957550452334E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-BB51-4C4B-8E1B-307D303008E1}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -2788,6 +3197,7 @@
                 <a:endParaRPr lang="it-IT"/>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="t"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -2817,9 +3227,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Pianificazione!$B$104:$B$107</c:f>
+              <c:f>Pianificazione!$B$104:$B$111</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>A</c:v>
                 </c:pt>
@@ -2827,25 +3237,55 @@
                   <c:v>PA</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>PD</c:v>
+                  <c:v>Incremento 5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>VC</c:v>
+                  <c:v>Incremento 6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Incremento 7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Incremento 8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Incremento 9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Incremento 10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Pianificazione!$C$104:$C$107</c:f>
+              <c:f>Pianificazione!$C$104:$C$111</c:f>
               <c:numCache>
                 <c:formatCode>#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-129</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2935,7 +3375,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -2980,7 +3420,6 @@
         <c:axId val="365909112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="90"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3348,10 +3787,10 @@
                   <c:v>PA</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>PD</c:v>
+                  <c:v>Incremento 5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>VC</c:v>
+                  <c:v>Incremento 6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3433,10 +3872,10 @@
                   <c:v>PA</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>PD</c:v>
+                  <c:v>Incremento 5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>VC</c:v>
+                  <c:v>Incremento 6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3507,10 +3946,10 @@
                   <c:v>PA</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>PD</c:v>
+                  <c:v>Incremento 5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>VC</c:v>
+                  <c:v>Incremento 6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7195,15 +7634,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1684020</xdr:colOff>
-      <xdr:row>73</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>145080</xdr:colOff>
-      <xdr:row>92</xdr:row>
-      <xdr:rowOff>4560</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>152700</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>103620</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7611,10 +8050,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EEB098D-590A-4332-807C-B47041EA10F7}">
-  <dimension ref="B4:F107"/>
+  <dimension ref="B4:F112"/>
   <sheetViews>
-    <sheetView topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="E89" sqref="E89"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -7630,457 +8069,864 @@
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="2:6">
-      <c r="B5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="B5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:6">
-      <c r="B6" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="9">
+      <c r="B6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="7">
         <v>0</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="7">
         <v>13154</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="7">
         <v>0</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:6">
-      <c r="B7" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="9">
+      <c r="B7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="7">
         <v>4417</v>
       </c>
-      <c r="D7" s="9">
-        <f>C13</f>
+      <c r="D7" s="7">
         <v>13154</v>
       </c>
-      <c r="E7" s="29">
+      <c r="E7" s="22">
         <f>F7</f>
         <v>4482</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="7">
         <v>4482</v>
       </c>
     </row>
     <row r="8" spans="2:6">
-      <c r="B8" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
+      <c r="B8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="7">
+        <v>967</v>
+      </c>
+      <c r="D8" s="7">
+        <v>13154</v>
+      </c>
+      <c r="E8" s="7">
+        <v>1007</v>
+      </c>
+      <c r="F8" s="7">
+        <v>1007</v>
+      </c>
     </row>
     <row r="9" spans="2:6">
-      <c r="B9" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="B9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="7">
+        <v>1326</v>
+      </c>
+      <c r="D9" s="7">
+        <v>13154</v>
+      </c>
+      <c r="E9" s="7">
+        <v>1197</v>
+      </c>
+      <c r="F9" s="7">
+        <v>1197</v>
+      </c>
     </row>
     <row r="10" spans="2:6">
-      <c r="B10" s="26"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
+      <c r="B10" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="7">
+        <v>1141</v>
+      </c>
+      <c r="D10" s="7">
+        <v>13154</v>
+      </c>
+      <c r="E10" s="7">
+        <f>F10</f>
+        <v>1441</v>
+      </c>
+      <c r="F10" s="7">
+        <v>1441</v>
+      </c>
     </row>
     <row r="11" spans="2:6">
-      <c r="B11" s="8"/>
+      <c r="B11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="7">
+        <v>1396</v>
+      </c>
+      <c r="D11" s="7">
+        <v>13154</v>
+      </c>
+      <c r="E11" s="7">
+        <f t="shared" ref="E11:E13" si="0">F11</f>
+        <v>1411</v>
+      </c>
+      <c r="F11" s="7">
+        <v>1411</v>
+      </c>
     </row>
     <row r="12" spans="2:6">
-      <c r="B12" s="13"/>
-      <c r="C12" s="12"/>
+      <c r="B12" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="7">
+        <v>521</v>
+      </c>
+      <c r="D12" s="7">
+        <v>13154</v>
+      </c>
+      <c r="E12" s="7">
+        <f t="shared" si="0"/>
+        <v>521</v>
+      </c>
+      <c r="F12" s="7">
+        <v>521</v>
+      </c>
     </row>
     <row r="13" spans="2:6">
-      <c r="B13" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="9">
+      <c r="B13" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="7">
+        <v>583</v>
+      </c>
+      <c r="D13" s="7">
         <v>13154</v>
+      </c>
+      <c r="E13" s="7">
+        <f t="shared" si="0"/>
+        <v>583</v>
+      </c>
+      <c r="F13" s="7">
+        <v>583</v>
       </c>
     </row>
     <row r="14" spans="2:6">
-      <c r="C14" s="14"/>
+      <c r="B14" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="10"/>
     </row>
     <row r="16" spans="2:6">
-      <c r="D16" s="15"/>
+      <c r="D16" s="11"/>
+    </row>
+    <row r="25" spans="2:6">
+      <c r="B25" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="7">
+        <v>13154</v>
+      </c>
     </row>
     <row r="27" spans="2:6">
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="2:6">
-      <c r="F28" s="16"/>
+      <c r="F28" s="12"/>
     </row>
     <row r="29" spans="2:6">
       <c r="B29" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
+        <v>9</v>
+      </c>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="17"/>
+      <c r="F29" s="13"/>
     </row>
     <row r="30" spans="2:6">
-      <c r="B30" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C30" s="4" t="s">
+      <c r="B30" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F30" s="20" t="s">
-        <v>25</v>
+      <c r="F30" s="16" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="2:6">
-      <c r="B31" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C31" s="9">
+      <c r="B31" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" s="7">
         <v>0</v>
       </c>
-      <c r="D31" s="9">
+      <c r="D31" s="7">
         <v>0</v>
       </c>
-      <c r="E31" s="9">
+      <c r="E31" s="7">
         <v>0</v>
       </c>
-      <c r="F31" s="9">
+      <c r="F31" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:6">
-      <c r="B32" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C32" s="9">
+      <c r="B32" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="7">
+        <f>C7</f>
         <v>4417</v>
       </c>
-      <c r="D32" s="9">
+      <c r="D32" s="7">
         <f>F32+(F32*5/100)</f>
         <v>4706.1000000000004</v>
       </c>
-      <c r="E32" s="9">
+      <c r="E32" s="7">
         <f>F32</f>
         <v>4482</v>
       </c>
-      <c r="F32" s="32">
+      <c r="F32" s="23">
         <f>F7</f>
         <v>4482</v>
       </c>
     </row>
     <row r="33" spans="2:6">
-      <c r="B33" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="28"/>
+      <c r="B33" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="7">
+        <f t="shared" ref="C33:C38" si="1">C8</f>
+        <v>967</v>
+      </c>
+      <c r="D33" s="7">
+        <f t="shared" ref="D33:D38" si="2">F33+(F33*5/100)</f>
+        <v>1057.3499999999999</v>
+      </c>
+      <c r="E33" s="7">
+        <f t="shared" ref="E33:E38" si="3">F33</f>
+        <v>1007</v>
+      </c>
+      <c r="F33" s="23">
+        <f>F8</f>
+        <v>1007</v>
+      </c>
     </row>
     <row r="34" spans="2:6">
-      <c r="B34" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34" s="3"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="28"/>
+      <c r="B34" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="7">
+        <f t="shared" si="1"/>
+        <v>1326</v>
+      </c>
+      <c r="D34" s="7">
+        <f t="shared" si="2"/>
+        <v>1256.8499999999999</v>
+      </c>
+      <c r="E34" s="7">
+        <f t="shared" si="3"/>
+        <v>1197</v>
+      </c>
+      <c r="F34" s="23">
+        <f>F9</f>
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6">
+      <c r="B35" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" s="7">
+        <f t="shared" si="1"/>
+        <v>1141</v>
+      </c>
+      <c r="D35" s="7">
+        <f t="shared" si="2"/>
+        <v>1513.05</v>
+      </c>
+      <c r="E35" s="7">
+        <f t="shared" si="3"/>
+        <v>1441</v>
+      </c>
+      <c r="F35" s="23">
+        <f t="shared" ref="F35:F38" si="4">F10</f>
+        <v>1441</v>
+      </c>
     </row>
     <row r="36" spans="2:6">
-      <c r="B36" s="16"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
+      <c r="B36" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" s="7">
+        <f t="shared" si="1"/>
+        <v>1396</v>
+      </c>
+      <c r="D36" s="7">
+        <f t="shared" si="2"/>
+        <v>1481.55</v>
+      </c>
+      <c r="E36" s="7">
+        <f t="shared" si="3"/>
+        <v>1411</v>
+      </c>
+      <c r="F36" s="23">
+        <f t="shared" si="4"/>
+        <v>1411</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6">
+      <c r="B37" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" s="7">
+        <f t="shared" si="1"/>
+        <v>521</v>
+      </c>
+      <c r="D37" s="7">
+        <f t="shared" si="2"/>
+        <v>547.04999999999995</v>
+      </c>
+      <c r="E37" s="7">
+        <f t="shared" si="3"/>
+        <v>521</v>
+      </c>
+      <c r="F37" s="23">
+        <f t="shared" si="4"/>
+        <v>521</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6">
+      <c r="B38" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" s="7">
+        <f t="shared" si="1"/>
+        <v>583</v>
+      </c>
+      <c r="D38" s="7">
+        <f t="shared" si="2"/>
+        <v>612.15</v>
+      </c>
+      <c r="E38" s="7">
+        <f t="shared" si="3"/>
+        <v>583</v>
+      </c>
+      <c r="F38" s="23">
+        <f t="shared" si="4"/>
+        <v>583</v>
+      </c>
     </row>
     <row r="59" spans="2:6">
       <c r="B59" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C59" s="6"/>
-      <c r="D59" s="6"/>
+        <v>6</v>
+      </c>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
       <c r="E59" s="1"/>
     </row>
     <row r="60" spans="2:6">
-      <c r="B60" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C60" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E60" s="16"/>
-      <c r="F60" s="21"/>
+      <c r="B60" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C60" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E60" s="12"/>
+      <c r="F60" s="17"/>
     </row>
     <row r="61" spans="2:6">
-      <c r="B61" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C61" s="37">
+      <c r="B61" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C61" s="27">
         <v>0</v>
       </c>
-      <c r="D61" s="32">
+      <c r="D61" s="23">
         <v>0</v>
       </c>
-      <c r="E61" s="17"/>
-      <c r="F61" s="17"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="13"/>
     </row>
     <row r="62" spans="2:6">
-      <c r="B62" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C62" s="40">
+      <c r="B62" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C62" s="29">
         <v>6.4999999999999997E-3</v>
       </c>
-      <c r="D62" s="39">
+      <c r="D62" s="28">
         <f>(F32-C32)/100</f>
         <v>0.65</v>
       </c>
-      <c r="E62" s="17"/>
-      <c r="F62" s="17"/>
+      <c r="E62" s="13"/>
+      <c r="F62" s="13"/>
     </row>
     <row r="63" spans="2:6">
-      <c r="B63" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="C63" s="38"/>
-      <c r="D63" s="32">
+      <c r="B63" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C63" s="29">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D63" s="28">
         <f>(F33-C33)/100</f>
-        <v>0</v>
-      </c>
-      <c r="E63" s="17"/>
-      <c r="F63" s="18"/>
+        <v>0.4</v>
+      </c>
+      <c r="E63" s="13"/>
+      <c r="F63" s="14"/>
     </row>
     <row r="64" spans="2:6">
-      <c r="B64" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C64" s="37"/>
-      <c r="D64" s="32">
-        <f>(F34-C34)/100</f>
-        <v>0</v>
-      </c>
-      <c r="E64" s="17"/>
-      <c r="F64" s="18"/>
+      <c r="B64" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C64" s="29">
+        <v>-1.29E-2</v>
+      </c>
+      <c r="D64" s="28">
+        <f t="shared" ref="D64:D67" si="5">(F34-C34)/100</f>
+        <v>-1.29</v>
+      </c>
+      <c r="E64" s="13"/>
+      <c r="F64" s="14"/>
     </row>
     <row r="65" spans="2:6">
-      <c r="B65" s="26"/>
-      <c r="C65" s="27"/>
-      <c r="D65" s="18"/>
-      <c r="E65" s="18"/>
-      <c r="F65" s="18"/>
+      <c r="B65" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C65" s="29">
+        <v>0.03</v>
+      </c>
+      <c r="D65" s="28">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14"/>
     </row>
     <row r="66" spans="2:6">
-      <c r="F66" s="18"/>
+      <c r="B66" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C66" s="29">
+        <v>1.5E-3</v>
+      </c>
+      <c r="D66" s="28">
+        <f t="shared" si="5"/>
+        <v>0.15</v>
+      </c>
+      <c r="F66" s="14"/>
+    </row>
+    <row r="67" spans="2:6">
+      <c r="B67" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C67" s="29">
+        <v>0</v>
+      </c>
+      <c r="D67" s="28">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6">
+      <c r="B68" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C68" s="29">
+        <v>0</v>
+      </c>
+      <c r="D68" s="28">
+        <f>(F38-C38)/100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6">
+      <c r="C69" s="29"/>
+      <c r="D69" s="28"/>
     </row>
     <row r="75" spans="2:6">
       <c r="B75" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C75" s="6"/>
+        <v>12</v>
+      </c>
+      <c r="C75" s="5"/>
     </row>
     <row r="76" spans="2:6">
-      <c r="B76" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C76" s="4" t="s">
+      <c r="B76" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D76" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D76" s="4" t="s">
+      <c r="E76" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="E76" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="77" spans="2:6">
-      <c r="B77" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C77" s="9">
+      <c r="B77" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C77" s="7">
         <v>0</v>
       </c>
-      <c r="D77" s="9">
+      <c r="D77" s="7">
         <v>0</v>
       </c>
-      <c r="E77" s="9">
+      <c r="E77" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="2:6">
-      <c r="B78" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C78" s="33">
+      <c r="B78" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C78" s="31">
         <f>E78-D78</f>
-        <v>-65</v>
-      </c>
-      <c r="D78" s="9">
+        <v>0</v>
+      </c>
+      <c r="D78" s="7">
+        <f>F32</f>
         <v>4482</v>
       </c>
-      <c r="E78" s="9">
-        <f>4482-65</f>
-        <v>4417</v>
+      <c r="E78" s="7">
+        <f>4482</f>
+        <v>4482</v>
       </c>
     </row>
     <row r="79" spans="2:6">
-      <c r="B79" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C79" s="33"/>
-      <c r="D79" s="31"/>
-      <c r="E79" s="30"/>
+      <c r="B79" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C79" s="31">
+        <f t="shared" ref="C79:C84" si="6">E79-D79</f>
+        <v>200</v>
+      </c>
+      <c r="D79" s="7">
+        <f t="shared" ref="D79:D83" si="7">F33</f>
+        <v>1007</v>
+      </c>
+      <c r="E79" s="7">
+        <f>1007+200</f>
+        <v>1207</v>
+      </c>
     </row>
     <row r="80" spans="2:6">
-      <c r="B80" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C80" s="33"/>
-      <c r="D80" s="31"/>
-      <c r="E80" s="30"/>
+      <c r="B80" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C80" s="31">
+        <f t="shared" si="6"/>
+        <v>300</v>
+      </c>
+      <c r="D80" s="7">
+        <f t="shared" si="7"/>
+        <v>1197</v>
+      </c>
+      <c r="E80" s="7">
+        <f>1197+300</f>
+        <v>1497</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5">
+      <c r="B81" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C81" s="31">
+        <f t="shared" si="6"/>
+        <v>-35</v>
+      </c>
+      <c r="D81" s="7">
+        <f t="shared" si="7"/>
+        <v>1441</v>
+      </c>
+      <c r="E81" s="7">
+        <f>1141+265</f>
+        <v>1406</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5">
+      <c r="B82" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C82" s="31">
+        <f t="shared" si="6"/>
+        <v>50</v>
+      </c>
+      <c r="D82" s="7">
+        <f t="shared" si="7"/>
+        <v>1411</v>
+      </c>
+      <c r="E82" s="7">
+        <f>1411+50</f>
+        <v>1461</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5">
+      <c r="B83" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C83" s="31">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D83" s="7">
+        <f t="shared" si="7"/>
+        <v>521</v>
+      </c>
+      <c r="E83" s="7">
+        <f>521</f>
+        <v>521</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5">
+      <c r="B84" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C84" s="31">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="D84" s="7">
+        <f>F38</f>
+        <v>583</v>
+      </c>
+      <c r="E84" s="7">
+        <f>583+10</f>
+        <v>593</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5">
+      <c r="D85" s="7"/>
     </row>
     <row r="92" spans="2:5">
-      <c r="B92" s="34"/>
-      <c r="C92" s="16"/>
-      <c r="D92" s="18"/>
-      <c r="E92" s="18"/>
+      <c r="B92" s="24"/>
+      <c r="C92" s="12"/>
+      <c r="D92" s="14"/>
+      <c r="E92" s="14"/>
     </row>
     <row r="93" spans="2:5">
-      <c r="B93" s="16"/>
-      <c r="C93" s="16"/>
-      <c r="D93" s="16"/>
-      <c r="E93" s="16"/>
+      <c r="B93" s="12"/>
+      <c r="C93" s="12"/>
+      <c r="D93" s="12"/>
+      <c r="E93" s="12"/>
     </row>
     <row r="94" spans="2:5">
-      <c r="B94" s="26"/>
-      <c r="C94" s="17"/>
-      <c r="D94" s="17"/>
-      <c r="E94" s="17"/>
+      <c r="B94" s="21"/>
+      <c r="C94" s="13"/>
+      <c r="D94" s="13"/>
+      <c r="E94" s="13"/>
     </row>
     <row r="95" spans="2:5">
-      <c r="B95" s="26"/>
-      <c r="C95" s="17"/>
-      <c r="D95" s="17"/>
-      <c r="E95" s="17"/>
+      <c r="B95" s="21"/>
+      <c r="C95" s="13"/>
+      <c r="D95" s="13"/>
+      <c r="E95" s="13"/>
     </row>
     <row r="96" spans="2:5">
-      <c r="B96" s="26"/>
-      <c r="C96" s="17"/>
-      <c r="D96" s="35"/>
-      <c r="E96" s="17"/>
+      <c r="B96" s="21"/>
+      <c r="C96" s="13"/>
+      <c r="D96" s="25"/>
+      <c r="E96" s="13"/>
     </row>
     <row r="97" spans="2:5">
-      <c r="B97" s="26"/>
-      <c r="C97" s="17"/>
-      <c r="D97" s="35"/>
-      <c r="E97" s="17"/>
+      <c r="B97" s="21"/>
+      <c r="C97" s="13"/>
+      <c r="D97" s="25"/>
+      <c r="E97" s="13"/>
     </row>
     <row r="102" spans="2:5">
       <c r="B102" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C102" s="6"/>
+        <v>16</v>
+      </c>
+      <c r="C102" s="5"/>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
     </row>
     <row r="103" spans="2:5">
-      <c r="B103" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C103" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D103" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E103" s="4" t="s">
-        <v>5</v>
+      <c r="B103" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E103" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="104" spans="2:5">
-      <c r="B104" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C104" s="9">
+      <c r="B104" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C104" s="7">
         <v>0</v>
       </c>
-      <c r="D104" s="9">
+      <c r="D104" s="7">
         <v>0</v>
       </c>
-      <c r="E104" s="9">
+      <c r="E104" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="105" spans="2:5">
-      <c r="B105" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C105" s="9">
+      <c r="B105" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C105" s="7">
         <f>D105-E105</f>
         <v>65</v>
       </c>
-      <c r="D105" s="9">
+      <c r="D105" s="7">
         <f>F7</f>
         <v>4482</v>
       </c>
-      <c r="E105" s="9">
+      <c r="E105" s="7">
         <f>C7</f>
         <v>4417</v>
       </c>
     </row>
     <row r="106" spans="2:5">
-      <c r="B106" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C106" s="33"/>
-      <c r="D106" s="31"/>
-      <c r="E106" s="30"/>
+      <c r="B106" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C106" s="7">
+        <f t="shared" ref="C106:C111" si="8">D106-E106</f>
+        <v>40</v>
+      </c>
+      <c r="D106" s="7">
+        <f t="shared" ref="D106:D110" si="9">F8</f>
+        <v>1007</v>
+      </c>
+      <c r="E106" s="7">
+        <f t="shared" ref="E106:E111" si="10">C8</f>
+        <v>967</v>
+      </c>
     </row>
     <row r="107" spans="2:5">
-      <c r="B107" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C107" s="33"/>
-      <c r="D107" s="31"/>
-      <c r="E107" s="30"/>
+      <c r="B107" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C107" s="7">
+        <f t="shared" si="8"/>
+        <v>-129</v>
+      </c>
+      <c r="D107" s="7">
+        <f t="shared" si="9"/>
+        <v>1197</v>
+      </c>
+      <c r="E107" s="7">
+        <f t="shared" si="10"/>
+        <v>1326</v>
+      </c>
+    </row>
+    <row r="108" spans="2:5">
+      <c r="B108" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C108" s="7">
+        <f t="shared" si="8"/>
+        <v>300</v>
+      </c>
+      <c r="D108" s="7">
+        <f t="shared" si="9"/>
+        <v>1441</v>
+      </c>
+      <c r="E108" s="7">
+        <f t="shared" si="10"/>
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="109" spans="2:5">
+      <c r="B109" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C109" s="7">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+      <c r="D109" s="7">
+        <f t="shared" si="9"/>
+        <v>1411</v>
+      </c>
+      <c r="E109" s="7">
+        <f t="shared" si="10"/>
+        <v>1396</v>
+      </c>
+    </row>
+    <row r="110" spans="2:5">
+      <c r="B110" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C110" s="7">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="D110" s="7">
+        <f t="shared" si="9"/>
+        <v>521</v>
+      </c>
+      <c r="E110" s="7">
+        <f t="shared" si="10"/>
+        <v>521</v>
+      </c>
+    </row>
+    <row r="111" spans="2:5">
+      <c r="B111" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C111" s="7">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="D111" s="7">
+        <f>F13</f>
+        <v>583</v>
+      </c>
+      <c r="E111" s="7">
+        <f t="shared" si="10"/>
+        <v>583</v>
+      </c>
+    </row>
+    <row r="112" spans="2:5">
+      <c r="D112" s="7"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -8091,8 +8937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A007753-E669-4835-90BB-B57BBACA4DE7}">
   <dimension ref="C5:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8107,124 +8953,144 @@
   <sheetData>
     <row r="5" spans="3:8">
       <c r="C5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
+        <v>20</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="17"/>
+      <c r="G5" s="13"/>
     </row>
     <row r="6" spans="3:8">
-      <c r="C6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="C6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7" spans="3:8">
-      <c r="C7" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="19">
+      <c r="C7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="15">
         <f>G7/H7</f>
         <v>1</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="15">
         <v>0.6</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F7" s="15">
         <v>0.8</v>
       </c>
-      <c r="G7" s="24">
+      <c r="G7" s="20">
         <v>3</v>
       </c>
-      <c r="H7" s="24">
+      <c r="H7" s="20">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="3:8">
-      <c r="C8" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="19">
+      <c r="C8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="15">
         <f>G8/H8</f>
         <v>1</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="15">
         <v>0.6</v>
       </c>
-      <c r="F8" s="19">
+      <c r="F8" s="15">
         <v>0.8</v>
       </c>
-      <c r="G8" s="24">
+      <c r="G8" s="20">
         <v>8</v>
       </c>
-      <c r="H8" s="24">
+      <c r="H8" s="20">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="3:8">
-      <c r="C9" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="19">
+      <c r="C9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="15">
         <f>G9/H9</f>
         <v>0.90476190476190477</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="15">
         <v>0.6</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="15">
         <v>0.8</v>
       </c>
-      <c r="G9" s="24">
+      <c r="G9" s="20">
         <v>19</v>
       </c>
-      <c r="H9" s="24">
+      <c r="H9" s="20">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="3:8">
-      <c r="C10" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="19">
+      <c r="C10" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="19"/>
+      <c r="E10" s="15">
         <v>0.6</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="15">
         <v>0.8</v>
       </c>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
     </row>
     <row r="11" spans="3:8">
-      <c r="G11" s="18"/>
+      <c r="C11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="3:8">
+      <c r="C12" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8">
+      <c r="C13" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8">
+      <c r="C14" s="30" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="15" spans="3:8">
-      <c r="C15" s="15"/>
+      <c r="C15" s="30" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="17" spans="6:6">
-      <c r="F17" s="15"/>
+      <c r="F17" s="11"/>
     </row>
     <row r="19" spans="6:6">
-      <c r="F19" s="15"/>
+      <c r="F19" s="11"/>
     </row>
     <row r="21" spans="6:6">
-      <c r="F21" s="15"/>
+      <c r="F21" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Spostata PMS, fix grafico PMS
</commit_message>
<xml_diff>
--- a/DocumentazioneEsterna/PianoDiQualifica/res/ResocontoAttivitaDiVerifica/res/metriche/grafici/qualitàProcesso/graficiProcessiOrganizzativi.xlsx
+++ b/DocumentazioneEsterna/PianoDiQualifica/res/ResocontoAttivitaDiVerifica/res/metriche/grafici/qualitàProcesso/graficiProcessiOrganizzativi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Università\Terzo anno\SWE\Progetto\Documentazione\DocumentazioneEsterna\PianoDiQualifica\res\ResocontoAttivitaDiVerifica\res\metriche\grafici\qualitàProcesso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9BBC95-42CF-470F-AF2A-4CDF15EE1399}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8993A93B-D998-4FB2-885D-F22BB59D8E93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{32F62035-8081-4F2C-A1C6-0EA80AA4F9D3}"/>
+    <workbookView xWindow="-7812" yWindow="2784" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{32F62035-8081-4F2C-A1C6-0EA80AA4F9D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Pianificazione" sheetId="1" r:id="rId1"/>
@@ -143,7 +143,7 @@
     <numFmt numFmtId="5" formatCode="&quot;€&quot;\ #,##0;\-&quot;€&quot;\ #,##0"/>
     <numFmt numFmtId="164" formatCode="#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]"/>
     <numFmt numFmtId="165" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
-    <numFmt numFmtId="167" formatCode="#,##0.00\ [$€-1];[Red]\-#,##0.00\ [$€-1]"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00\ [$€-1];[Red]\-#,##0.00\ [$€-1]"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -292,7 +292,6 @@
     <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -301,10 +300,11 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="5" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -3777,9 +3777,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>GestioneQualità!$C$7:$C$10</c:f>
+              <c:f>GestioneQualità!$C$7:$C$15</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>A</c:v>
                 </c:pt>
@@ -3791,16 +3791,31 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Incremento 6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Incremento 7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Incremento 8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Incremento 9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Incremento 10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>PD</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>GestioneQualità!$D$7:$D$10</c:f>
+              <c:f>GestioneQualità!$D$7:$D$15</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3808,7 +3823,25 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.90476190476190477</c:v>
+                  <c:v>0.94444444444444442</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.83333333333333337</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.88888888888888884</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.88888888888888884</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.88888888888888884</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.94736842105263153</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3862,9 +3895,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>GestioneQualità!$C$7:$C$10</c:f>
+              <c:f>GestioneQualità!$C$7:$C$15</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>A</c:v>
                 </c:pt>
@@ -3876,16 +3909,31 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Incremento 6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Incremento 7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Incremento 8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Incremento 9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Incremento 10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>PD</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>GestioneQualità!$E$7:$E$10</c:f>
+              <c:f>GestioneQualità!$E$7:$E$15</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.6</c:v>
                 </c:pt>
@@ -3896,6 +3944,21 @@
                   <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0.6</c:v>
                 </c:pt>
               </c:numCache>
@@ -3936,9 +3999,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>GestioneQualità!$C$7:$C$10</c:f>
+              <c:f>GestioneQualità!$C$7:$C$15</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>A</c:v>
                 </c:pt>
@@ -3950,16 +4013,31 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Incremento 6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Incremento 7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Incremento 8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Incremento 9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Incremento 10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>PD</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>GestioneQualità!$F$7:$F$10</c:f>
+              <c:f>GestioneQualità!$F$7:$F$15</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.8</c:v>
                 </c:pt>
@@ -3970,6 +4048,21 @@
                   <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0.8</c:v>
                 </c:pt>
               </c:numCache>
@@ -8117,7 +8210,7 @@
       <c r="D7" s="7">
         <v>13154</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="21">
         <f>F7</f>
         <v>4482</v>
       </c>
@@ -8214,7 +8307,7 @@
       </c>
     </row>
     <row r="13" spans="2:6">
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="29" t="s">
         <v>32</v>
       </c>
       <c r="C13" s="7">
@@ -8232,7 +8325,7 @@
       </c>
     </row>
     <row r="14" spans="2:6">
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="29" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="10"/>
@@ -8313,7 +8406,7 @@
         <f>F32</f>
         <v>4482</v>
       </c>
-      <c r="F32" s="23">
+      <c r="F32" s="22">
         <f>F7</f>
         <v>4482</v>
       </c>
@@ -8334,7 +8427,7 @@
         <f t="shared" ref="E33:E38" si="3">F33</f>
         <v>1007</v>
       </c>
-      <c r="F33" s="23">
+      <c r="F33" s="22">
         <f>F8</f>
         <v>1007</v>
       </c>
@@ -8355,7 +8448,7 @@
         <f t="shared" si="3"/>
         <v>1197</v>
       </c>
-      <c r="F34" s="23">
+      <c r="F34" s="22">
         <f>F9</f>
         <v>1197</v>
       </c>
@@ -8376,7 +8469,7 @@
         <f t="shared" si="3"/>
         <v>1441</v>
       </c>
-      <c r="F35" s="23">
+      <c r="F35" s="22">
         <f t="shared" ref="F35:F38" si="4">F10</f>
         <v>1441</v>
       </c>
@@ -8397,7 +8490,7 @@
         <f t="shared" si="3"/>
         <v>1411</v>
       </c>
-      <c r="F36" s="23">
+      <c r="F36" s="22">
         <f t="shared" si="4"/>
         <v>1411</v>
       </c>
@@ -8418,13 +8511,13 @@
         <f t="shared" si="3"/>
         <v>521</v>
       </c>
-      <c r="F37" s="23">
+      <c r="F37" s="22">
         <f t="shared" si="4"/>
         <v>521</v>
       </c>
     </row>
     <row r="38" spans="2:6">
-      <c r="B38" s="30" t="s">
+      <c r="B38" s="29" t="s">
         <v>32</v>
       </c>
       <c r="C38" s="7">
@@ -8439,7 +8532,7 @@
         <f t="shared" si="3"/>
         <v>583</v>
       </c>
-      <c r="F38" s="23">
+      <c r="F38" s="22">
         <f t="shared" si="4"/>
         <v>583</v>
       </c>
@@ -8456,7 +8549,7 @@
       <c r="B60" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C60" s="26" t="s">
+      <c r="C60" s="25" t="s">
         <v>8</v>
       </c>
       <c r="D60" s="3" t="s">
@@ -8469,10 +8562,10 @@
       <c r="B61" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C61" s="27">
+      <c r="C61" s="26">
         <v>0</v>
       </c>
-      <c r="D61" s="23">
+      <c r="D61" s="22">
         <v>0</v>
       </c>
       <c r="E61" s="13"/>
@@ -8482,10 +8575,10 @@
       <c r="B62" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C62" s="29">
+      <c r="C62" s="28">
         <v>6.4999999999999997E-3</v>
       </c>
-      <c r="D62" s="28">
+      <c r="D62" s="27">
         <f>(F32-C32)/100</f>
         <v>0.65</v>
       </c>
@@ -8496,10 +8589,10 @@
       <c r="B63" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C63" s="29">
+      <c r="C63" s="28">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D63" s="28">
+      <c r="D63" s="27">
         <f>(F33-C33)/100</f>
         <v>0.4</v>
       </c>
@@ -8510,10 +8603,10 @@
       <c r="B64" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C64" s="29">
+      <c r="C64" s="28">
         <v>-1.29E-2</v>
       </c>
-      <c r="D64" s="28">
+      <c r="D64" s="27">
         <f t="shared" ref="D64:D67" si="5">(F34-C34)/100</f>
         <v>-1.29</v>
       </c>
@@ -8524,10 +8617,10 @@
       <c r="B65" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C65" s="29">
+      <c r="C65" s="28">
         <v>0.03</v>
       </c>
-      <c r="D65" s="28">
+      <c r="D65" s="27">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
@@ -8538,10 +8631,10 @@
       <c r="B66" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C66" s="29">
+      <c r="C66" s="28">
         <v>1.5E-3</v>
       </c>
-      <c r="D66" s="28">
+      <c r="D66" s="27">
         <f t="shared" si="5"/>
         <v>0.15</v>
       </c>
@@ -8551,29 +8644,29 @@
       <c r="B67" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C67" s="29">
+      <c r="C67" s="28">
         <v>0</v>
       </c>
-      <c r="D67" s="28">
+      <c r="D67" s="27">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="2:6">
-      <c r="B68" s="30" t="s">
+      <c r="B68" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C68" s="29">
+      <c r="C68" s="28">
         <v>0</v>
       </c>
-      <c r="D68" s="28">
+      <c r="D68" s="27">
         <f>(F38-C38)/100</f>
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="2:6">
-      <c r="C69" s="29"/>
-      <c r="D69" s="28"/>
+      <c r="C69" s="28"/>
+      <c r="D69" s="27"/>
     </row>
     <row r="75" spans="2:6">
       <c r="B75" s="2" t="s">
@@ -8613,7 +8706,7 @@
       <c r="B78" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C78" s="31">
+      <c r="C78" s="30">
         <f>E78-D78</f>
         <v>0</v>
       </c>
@@ -8630,7 +8723,7 @@
       <c r="B79" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C79" s="31">
+      <c r="C79" s="30">
         <f t="shared" ref="C79:C84" si="6">E79-D79</f>
         <v>200</v>
       </c>
@@ -8647,7 +8740,7 @@
       <c r="B80" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C80" s="31">
+      <c r="C80" s="30">
         <f t="shared" si="6"/>
         <v>300</v>
       </c>
@@ -8664,7 +8757,7 @@
       <c r="B81" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C81" s="31">
+      <c r="C81" s="30">
         <f t="shared" si="6"/>
         <v>-35</v>
       </c>
@@ -8681,7 +8774,7 @@
       <c r="B82" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C82" s="31">
+      <c r="C82" s="30">
         <f t="shared" si="6"/>
         <v>50</v>
       </c>
@@ -8698,7 +8791,7 @@
       <c r="B83" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C83" s="31">
+      <c r="C83" s="30">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -8712,10 +8805,10 @@
       </c>
     </row>
     <row r="84" spans="2:5">
-      <c r="B84" s="30" t="s">
+      <c r="B84" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C84" s="31">
+      <c r="C84" s="30">
         <f t="shared" si="6"/>
         <v>10</v>
       </c>
@@ -8732,7 +8825,7 @@
       <c r="D85" s="7"/>
     </row>
     <row r="92" spans="2:5">
-      <c r="B92" s="24"/>
+      <c r="B92" s="23"/>
       <c r="C92" s="12"/>
       <c r="D92" s="14"/>
       <c r="E92" s="14"/>
@@ -8744,27 +8837,27 @@
       <c r="E93" s="12"/>
     </row>
     <row r="94" spans="2:5">
-      <c r="B94" s="21"/>
+      <c r="B94" s="20"/>
       <c r="C94" s="13"/>
       <c r="D94" s="13"/>
       <c r="E94" s="13"/>
     </row>
     <row r="95" spans="2:5">
-      <c r="B95" s="21"/>
+      <c r="B95" s="20"/>
       <c r="C95" s="13"/>
       <c r="D95" s="13"/>
       <c r="E95" s="13"/>
     </row>
     <row r="96" spans="2:5">
-      <c r="B96" s="21"/>
+      <c r="B96" s="20"/>
       <c r="C96" s="13"/>
-      <c r="D96" s="25"/>
+      <c r="D96" s="24"/>
       <c r="E96" s="13"/>
     </row>
     <row r="97" spans="2:5">
-      <c r="B97" s="21"/>
+      <c r="B97" s="20"/>
       <c r="C97" s="13"/>
-      <c r="D97" s="25"/>
+      <c r="D97" s="24"/>
       <c r="E97" s="13"/>
     </row>
     <row r="102" spans="2:5">
@@ -8906,7 +8999,7 @@
       </c>
     </row>
     <row r="111" spans="2:5">
-      <c r="B111" s="30" t="s">
+      <c r="B111" s="29" t="s">
         <v>32</v>
       </c>
       <c r="C111" s="7">
@@ -8937,8 +9030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A007753-E669-4835-90BB-B57BBACA4DE7}">
   <dimension ref="C5:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:C15"/>
+    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8994,10 +9087,10 @@
       <c r="F7" s="15">
         <v>0.8</v>
       </c>
-      <c r="G7" s="20">
+      <c r="G7" s="19">
         <v>3</v>
       </c>
-      <c r="H7" s="20">
+      <c r="H7" s="19">
         <v>3</v>
       </c>
     </row>
@@ -9015,10 +9108,10 @@
       <c r="F8" s="15">
         <v>0.8</v>
       </c>
-      <c r="G8" s="20">
+      <c r="G8" s="19">
         <v>8</v>
       </c>
-      <c r="H8" s="20">
+      <c r="H8" s="19">
         <v>8</v>
       </c>
     </row>
@@ -9028,7 +9121,7 @@
       </c>
       <c r="D9" s="15">
         <f>G9/H9</f>
-        <v>0.90476190476190477</v>
+        <v>0.94444444444444442</v>
       </c>
       <c r="E9" s="15">
         <v>0.6</v>
@@ -9036,51 +9129,137 @@
       <c r="F9" s="15">
         <v>0.8</v>
       </c>
-      <c r="G9" s="20">
-        <v>19</v>
-      </c>
-      <c r="H9" s="20">
-        <v>21</v>
+      <c r="G9" s="19">
+        <v>17</v>
+      </c>
+      <c r="H9" s="19">
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="3:8">
       <c r="C10" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="19"/>
+      <c r="D10" s="15">
+        <f t="shared" ref="D10:D15" si="0">G10/H10</f>
+        <v>0.66666666666666663</v>
+      </c>
       <c r="E10" s="15">
         <v>0.6</v>
       </c>
       <c r="F10" s="15">
         <v>0.8</v>
       </c>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
+      <c r="G10" s="19">
+        <v>12</v>
+      </c>
+      <c r="H10" s="19">
+        <v>18</v>
+      </c>
     </row>
     <row r="11" spans="3:8">
       <c r="C11" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="14"/>
+      <c r="D11" s="15">
+        <f t="shared" si="0"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E11" s="15">
+        <v>0.6</v>
+      </c>
+      <c r="F11" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="G11" s="31">
+        <v>15</v>
+      </c>
+      <c r="H11" s="19">
+        <v>18</v>
+      </c>
     </row>
     <row r="12" spans="3:8">
       <c r="C12" s="8" t="s">
         <v>30</v>
       </c>
+      <c r="D12" s="15">
+        <f t="shared" si="0"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="E12" s="15">
+        <v>0.6</v>
+      </c>
+      <c r="F12" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="G12" s="31">
+        <v>16</v>
+      </c>
+      <c r="H12" s="19">
+        <v>18</v>
+      </c>
     </row>
     <row r="13" spans="3:8">
       <c r="C13" s="8" t="s">
         <v>31</v>
       </c>
+      <c r="D13" s="15">
+        <f t="shared" si="0"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="E13" s="15">
+        <v>0.6</v>
+      </c>
+      <c r="F13" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="G13" s="31">
+        <v>16</v>
+      </c>
+      <c r="H13" s="19">
+        <v>18</v>
+      </c>
     </row>
     <row r="14" spans="3:8">
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="29" t="s">
         <v>32</v>
+      </c>
+      <c r="D14" s="15">
+        <f t="shared" si="0"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="E14" s="15">
+        <v>0.6</v>
+      </c>
+      <c r="F14" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="G14" s="31">
+        <v>16</v>
+      </c>
+      <c r="H14" s="19">
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="3:8">
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="29" t="s">
         <v>3</v>
+      </c>
+      <c r="D15" s="15">
+        <f t="shared" si="0"/>
+        <v>0.94736842105263153</v>
+      </c>
+      <c r="E15" s="15">
+        <v>0.6</v>
+      </c>
+      <c r="F15" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="G15" s="31">
+        <v>18</v>
+      </c>
+      <c r="H15" s="19">
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="6:6">

</xml_diff>

<commit_message>
Last fix dati grafici
</commit_message>
<xml_diff>
--- a/DocumentazioneEsterna/PianoDiQualifica/res/ResocontoAttivitaDiVerifica/res/metriche/grafici/qualitàProcesso/graficiProcessiOrganizzativi.xlsx
+++ b/DocumentazioneEsterna/PianoDiQualifica/res/ResocontoAttivitaDiVerifica/res/metriche/grafici/qualitàProcesso/graficiProcessiOrganizzativi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Università\Terzo anno\SWE\Progetto\Documentazione\DocumentazioneEsterna\PianoDiQualifica\res\ResocontoAttivitaDiVerifica\res\metriche\grafici\qualitàProcesso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10498D1-0CA6-4A0F-9E10-47C3BF1F8774}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A48356-5DD5-4302-A683-31299272359F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{32F62035-8081-4F2C-A1C6-0EA80AA4F9D3}"/>
   </bookViews>
@@ -767,7 +767,7 @@
                   <c:v>521</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>583</c:v>
+                  <c:v>568</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1559,7 +1559,7 @@
                   <c:v>521</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>583</c:v>
+                  <c:v>568</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2160,7 +2160,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1.5E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3285,7 +3285,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8127,8 +8127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EEB098D-590A-4332-807C-B47041EA10F7}">
   <dimension ref="B4:F112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="F103" sqref="F103"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="D115" sqref="D115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8293,7 +8293,7 @@
         <v>32</v>
       </c>
       <c r="C13" s="7">
-        <v>583</v>
+        <v>568</v>
       </c>
       <c r="D13" s="7">
         <v>13154</v>
@@ -8507,7 +8507,7 @@
       </c>
       <c r="C38" s="7">
         <f t="shared" si="1"/>
-        <v>583</v>
+        <v>568</v>
       </c>
       <c r="D38" s="7">
         <f t="shared" si="2"/>
@@ -8642,11 +8642,11 @@
         <v>32</v>
       </c>
       <c r="C68" s="28">
-        <v>0</v>
+        <v>1.5E-3</v>
       </c>
       <c r="D68" s="27">
         <f>(F38-C38)/100</f>
-        <v>0</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="69" spans="2:6">
@@ -8989,7 +8989,7 @@
       </c>
       <c r="C111" s="7">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D111" s="7">
         <f>F13</f>
@@ -8997,7 +8997,7 @@
       </c>
       <c r="E111" s="7">
         <f t="shared" si="10"/>
-        <v>583</v>
+        <v>568</v>
       </c>
     </row>
     <row r="112" spans="2:5">

</xml_diff>

<commit_message>
Setup grafici per prossimi incrementi
</commit_message>
<xml_diff>
--- a/DocumentazioneEsterna/PianoDiQualifica/res/ResocontoAttivitaDiVerifica/res/metriche/grafici/qualitàProcesso/graficiProcessiOrganizzativi.xlsx
+++ b/DocumentazioneEsterna/PianoDiQualifica/res/ResocontoAttivitaDiVerifica/res/metriche/grafici/qualitàProcesso/graficiProcessiOrganizzativi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Università\Terzo anno\SWE\Progetto\Documentazione\DocumentazioneEsterna\PianoDiQualifica\res\ResocontoAttivitaDiVerifica\res\metriche\grafici\qualitàProcesso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A48356-5DD5-4302-A683-31299272359F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D94D8E-B6E8-49F8-ACF5-87FDBD30597E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{32F62035-8081-4F2C-A1C6-0EA80AA4F9D3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{32F62035-8081-4F2C-A1C6-0EA80AA4F9D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Pianificazione" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="35">
   <si>
     <t>Accettabile</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>Actual cost</t>
-  </si>
-  <si>
-    <t>PD</t>
   </si>
   <si>
     <t>AC</t>
@@ -134,6 +131,15 @@
   <si>
     <t>Incremento 10</t>
   </si>
+  <si>
+    <t>Incremento 11</t>
+  </si>
+  <si>
+    <t>Incremento 12</t>
+  </si>
+  <si>
+    <t>Incremento 13</t>
+  </si>
 </sst>
 </file>
 
@@ -145,7 +151,7 @@
     <numFmt numFmtId="165" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
     <numFmt numFmtId="166" formatCode="#,##0.00\ [$€-1];[Red]\-#,##0.00\ [$€-1]"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,11 +174,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Docs-Calibri"/>
     </font>
     <font>
       <u/>
@@ -272,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -283,8 +284,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -433,9 +433,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Pianificazione!$B$6:$B$13</c:f>
+              <c:f>Pianificazione!$B$6:$B$16</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>A</c:v>
                 </c:pt>
@@ -459,16 +459,25 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Incremento 10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Incremento 11</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Incremento 12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Incremento 13</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Pianificazione!$D$6:$D$13</c:f>
+              <c:f>Pianificazione!$D$6:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>13154</c:v>
                 </c:pt>
@@ -491,6 +500,15 @@
                   <c:v>13154</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>13154</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13154</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13154</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>13154</c:v>
                 </c:pt>
               </c:numCache>
@@ -530,9 +548,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Pianificazione!$B$6:$B$13</c:f>
+              <c:f>Pianificazione!$B$6:$B$16</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>A</c:v>
                 </c:pt>
@@ -556,16 +574,25 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Incremento 10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Incremento 11</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Incremento 12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Incremento 13</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Pianificazione!$E$6:$E$13</c:f>
+              <c:f>Pianificazione!$E$6:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -589,6 +616,15 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>583</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>584</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>585</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>586</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -709,9 +745,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Pianificazione!$B$6:$B$13</c:f>
+              <c:f>Pianificazione!$B$6:$B$16</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>A</c:v>
                 </c:pt>
@@ -735,16 +771,25 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Incremento 10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Incremento 11</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Incremento 12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Incremento 13</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Pianificazione!$C$6:$C$13</c:f>
+              <c:f>Pianificazione!$C$6:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -767,6 +812,15 @@
                   <c:v>521</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>568</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>568</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>568</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>568</c:v>
                 </c:pt>
               </c:numCache>
@@ -1201,9 +1255,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Pianificazione!$B$31:$B$38</c:f>
+              <c:f>Pianificazione!$B$31:$B$41</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>A</c:v>
                 </c:pt>
@@ -1227,16 +1281,25 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Incremento 10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Incremento 11</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Incremento 12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Incremento 13</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Pianificazione!$D$31:$D$38</c:f>
+              <c:f>Pianificazione!$D$31:$D$41</c:f>
               <c:numCache>
                 <c:formatCode>#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1260,6 +1323,15 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>612.15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>613.20000000000005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>614.25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>615.29999999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1298,9 +1370,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Pianificazione!$B$31:$B$38</c:f>
+              <c:f>Pianificazione!$B$31:$B$41</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>A</c:v>
                 </c:pt>
@@ -1324,16 +1396,25 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Incremento 10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Incremento 11</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Incremento 12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Incremento 13</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Pianificazione!$E$31:$E$38</c:f>
+              <c:f>Pianificazione!$E$31:$E$41</c:f>
               <c:numCache>
                 <c:formatCode>#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1357,6 +1438,15 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>583</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>584</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>585</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>586</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1501,9 +1591,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Pianificazione!$B$31:$B$38</c:f>
+              <c:f>Pianificazione!$B$31:$B$41</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>A</c:v>
                 </c:pt>
@@ -1527,16 +1617,25 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Incremento 10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Incremento 11</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Incremento 12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Incremento 13</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Pianificazione!$C$31:$C$38</c:f>
+              <c:f>Pianificazione!$C$31:$C$41</c:f>
               <c:numCache>
                 <c:formatCode>#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1559,6 +1658,15 @@
                   <c:v>521</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>568</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>568</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>568</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>568</c:v>
                 </c:pt>
               </c:numCache>
@@ -2102,9 +2210,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Pianificazione!$B$61:$B$68</c:f>
+              <c:f>Pianificazione!$B$61:$B$71</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>A</c:v>
                 </c:pt>
@@ -2128,16 +2236,25 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Incremento 10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Incremento 11</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Incremento 12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Incremento 13</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Pianificazione!$C$61:$C$68</c:f>
+              <c:f>Pianificazione!$C$61:$C$71</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="0%">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2161,6 +2278,15 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1.5E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0015000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.0015000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.0015000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2626,9 +2752,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Pianificazione!$B$77:$B$84</c:f>
+              <c:f>Pianificazione!$B$77:$B$87</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>A</c:v>
                 </c:pt>
@@ -2652,16 +2778,25 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Incremento 10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Incremento 11</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Incremento 12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Incremento 13</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Pianificazione!$C$77:$C$84</c:f>
+              <c:f>Pianificazione!$C$77:$C$87</c:f>
               <c:numCache>
                 <c:formatCode>"€"#,##0_);\("€"#,##0\)</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2685,6 +2820,15 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3227,9 +3371,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Pianificazione!$B$104:$B$111</c:f>
+              <c:f>Pianificazione!$B$104:$B$114</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>A</c:v>
                 </c:pt>
@@ -3253,16 +3397,25 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Incremento 10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Incremento 11</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Incremento 12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Incremento 13</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Pianificazione!$C$104:$C$111</c:f>
+              <c:f>Pianificazione!$C$104:$C$114</c:f>
               <c:numCache>
                 <c:formatCode>#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3286,6 +3439,15 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3777,62 +3939,62 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>GestioneQualità!$C$7:$C$14</c:f>
+              <c:f>GestioneQualità!$C$10:$C$17</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>A</c:v>
+                  <c:v>Incremento 6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>PA</c:v>
+                  <c:v>Incremento 7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Incremento 5</c:v>
+                  <c:v>Incremento 8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Incremento 6</c:v>
+                  <c:v>Incremento 9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Incremento 7</c:v>
+                  <c:v>Incremento 10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Incremento 8</c:v>
+                  <c:v>Incremento 11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Incremento 9</c:v>
+                  <c:v>Incremento 12</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Incremento 10</c:v>
+                  <c:v>Incremento 13</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>GestioneQualità!$D$7:$D$14</c:f>
+              <c:f>GestioneQualità!$D$10:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0.77777777777777779</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.94444444444444442</c:v>
+                  <c:v>0.83333333333333337</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>0.83333333333333337</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.77777777777777779</c:v>
+                  <c:v>0.89473684210526316</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.83333333333333337</c:v>
+                  <c:v>0.89473684210526316</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.83333333333333337</c:v>
+                  <c:v>0.89473684210526316</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.89473684210526316</c:v>
@@ -3889,39 +4051,39 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>GestioneQualità!$C$7:$C$14</c:f>
+              <c:f>GestioneQualità!$C$10:$C$17</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>A</c:v>
+                  <c:v>Incremento 6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>PA</c:v>
+                  <c:v>Incremento 7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Incremento 5</c:v>
+                  <c:v>Incremento 8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Incremento 6</c:v>
+                  <c:v>Incremento 9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Incremento 7</c:v>
+                  <c:v>Incremento 10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Incremento 8</c:v>
+                  <c:v>Incremento 11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Incremento 9</c:v>
+                  <c:v>Incremento 12</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Incremento 10</c:v>
+                  <c:v>Incremento 13</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>GestioneQualità!$E$7:$E$14</c:f>
+              <c:f>GestioneQualità!$E$10:$E$17</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3987,39 +4149,39 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>GestioneQualità!$C$7:$C$14</c:f>
+              <c:f>GestioneQualità!$C$10:$C$17</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>A</c:v>
+                  <c:v>Incremento 6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>PA</c:v>
+                  <c:v>Incremento 7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Incremento 5</c:v>
+                  <c:v>Incremento 8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Incremento 6</c:v>
+                  <c:v>Incremento 9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Incremento 7</c:v>
+                  <c:v>Incremento 10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Incremento 8</c:v>
+                  <c:v>Incremento 11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Incremento 9</c:v>
+                  <c:v>Incremento 12</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Incremento 10</c:v>
+                  <c:v>Incremento 13</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>GestioneQualità!$F$7:$F$14</c:f>
+              <c:f>GestioneQualità!$F$10:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="8"/>
@@ -7789,16 +7951,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>434340</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1371600</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>137460</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>172200</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>564180</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>65520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8125,13 +8287,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EEB098D-590A-4332-807C-B47041EA10F7}">
-  <dimension ref="B4:F112"/>
+  <dimension ref="B4:F116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="D115" sqref="D115"/>
+    <sheetView topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="D116" sqref="D116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="26.33203125" customWidth="1"/>
     <col min="3" max="3" width="19.77734375" customWidth="1"/>
@@ -8140,7 +8302,7 @@
     <col min="6" max="6" width="25.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:6">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
@@ -8148,12 +8310,12 @@
       <c r="D4" s="5"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>0</v>
@@ -8162,12 +8324,12 @@
         <v>1</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="7">
         <v>0</v>
@@ -8182,9 +8344,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="7">
         <v>4417</v>
@@ -8192,7 +8354,7 @@
       <c r="D7" s="7">
         <v>13154</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="20">
         <f>F7</f>
         <v>4482</v>
       </c>
@@ -8200,9 +8362,9 @@
         <v>4482</v>
       </c>
     </row>
-    <row r="8" spans="2:6">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="7">
         <v>967</v>
@@ -8217,9 +8379,9 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="9" spans="2:6">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="7">
         <v>1326</v>
@@ -8234,9 +8396,9 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="10" spans="2:6">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="7">
         <v>1411</v>
@@ -8252,9 +8414,9 @@
         <v>1441</v>
       </c>
     </row>
-    <row r="11" spans="2:6">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="7">
         <v>1396</v>
@@ -8270,9 +8432,9 @@
         <v>1411</v>
       </c>
     </row>
-    <row r="12" spans="2:6">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" s="7">
         <v>521</v>
@@ -8288,9 +8450,9 @@
         <v>521</v>
       </c>
     </row>
-    <row r="13" spans="2:6">
-      <c r="B13" s="29" t="s">
-        <v>32</v>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B13" s="28" t="s">
+        <v>31</v>
       </c>
       <c r="C13" s="7">
         <v>568</v>
@@ -8306,61 +8468,106 @@
         <v>583</v>
       </c>
     </row>
-    <row r="14" spans="2:6">
-      <c r="B14" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="10"/>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B14" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="7">
+        <v>568</v>
+      </c>
+      <c r="D14" s="7">
+        <v>13154</v>
+      </c>
+      <c r="E14" s="7">
+        <f t="shared" ref="E14:E16" si="1">F14</f>
+        <v>584</v>
+      </c>
+      <c r="F14" s="7">
+        <v>584</v>
+      </c>
     </row>
-    <row r="16" spans="2:6">
-      <c r="D16" s="11"/>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B15" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="7">
+        <v>568</v>
+      </c>
+      <c r="D15" s="7">
+        <v>13154</v>
+      </c>
+      <c r="E15" s="7">
+        <f t="shared" si="1"/>
+        <v>585</v>
+      </c>
+      <c r="F15" s="7">
+        <v>585</v>
+      </c>
     </row>
-    <row r="18" spans="2:6">
-      <c r="D18" s="11"/>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B16" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="7">
+        <v>568</v>
+      </c>
+      <c r="D16" s="7">
+        <v>13154</v>
+      </c>
+      <c r="E16" s="7">
+        <f t="shared" si="1"/>
+        <v>586</v>
+      </c>
+      <c r="F16" s="7">
+        <v>586</v>
+      </c>
     </row>
-    <row r="25" spans="2:6">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D18" s="10"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C25" s="7">
         <v>13154</v>
       </c>
     </row>
-    <row r="27" spans="2:6">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="2:6">
-      <c r="F28" s="12"/>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F28" s="11"/>
     </row>
-    <row r="29" spans="2:6">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="13"/>
+      <c r="F29" s="12"/>
     </row>
-    <row r="30" spans="2:6">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C30" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F30" s="16" t="s">
-        <v>24</v>
+      <c r="F30" s="15" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="31" spans="2:6">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B31" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C31" s="7">
         <v>0</v>
@@ -8375,9 +8582,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:6">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B32" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C32" s="7">
         <f>C7</f>
@@ -8391,291 +8598,386 @@
         <f>F32</f>
         <v>4482</v>
       </c>
-      <c r="F32" s="22">
+      <c r="F32" s="21">
         <f>F7</f>
         <v>4482</v>
       </c>
     </row>
-    <row r="33" spans="2:6">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B33" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C33" s="7">
-        <f t="shared" ref="C33:C38" si="1">C8</f>
+        <f t="shared" ref="C33:C41" si="2">C8</f>
         <v>967</v>
       </c>
       <c r="D33" s="7">
-        <f t="shared" ref="D33:D38" si="2">F33+(F33*5/100)</f>
+        <f t="shared" ref="D33:D38" si="3">F33+(F33*5/100)</f>
         <v>1057.3499999999999</v>
       </c>
       <c r="E33" s="7">
-        <f t="shared" ref="E33:E38" si="3">F33</f>
+        <f t="shared" ref="E33:E38" si="4">F33</f>
         <v>1007</v>
       </c>
-      <c r="F33" s="22">
+      <c r="F33" s="21">
         <f>F8</f>
         <v>1007</v>
       </c>
     </row>
-    <row r="34" spans="2:6">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B34" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C34" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1326</v>
       </c>
       <c r="D34" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1256.8499999999999</v>
       </c>
       <c r="E34" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1197</v>
       </c>
-      <c r="F34" s="22">
+      <c r="F34" s="21">
         <f>F9</f>
         <v>1197</v>
       </c>
     </row>
-    <row r="35" spans="2:6">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B35" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" s="7">
+        <f t="shared" si="2"/>
+        <v>1411</v>
+      </c>
+      <c r="D35" s="7">
+        <f t="shared" si="3"/>
+        <v>1513.05</v>
+      </c>
+      <c r="E35" s="7">
+        <f t="shared" si="4"/>
+        <v>1441</v>
+      </c>
+      <c r="F35" s="21">
+        <f t="shared" ref="F35:F41" si="5">F10</f>
+        <v>1441</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B36" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C35" s="7">
-        <f t="shared" si="1"/>
-        <v>1411</v>
-      </c>
-      <c r="D35" s="7">
+      <c r="C36" s="7">
         <f t="shared" si="2"/>
-        <v>1513.05</v>
-      </c>
-      <c r="E35" s="7">
+        <v>1396</v>
+      </c>
+      <c r="D36" s="7">
         <f t="shared" si="3"/>
-        <v>1441</v>
-      </c>
-      <c r="F35" s="22">
-        <f t="shared" ref="F35:F38" si="4">F10</f>
-        <v>1441</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6">
-      <c r="B36" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C36" s="7">
-        <f t="shared" si="1"/>
-        <v>1396</v>
-      </c>
-      <c r="D36" s="7">
-        <f t="shared" si="2"/>
         <v>1481.55</v>
       </c>
       <c r="E36" s="7">
-        <f t="shared" si="3"/>
-        <v>1411</v>
-      </c>
-      <c r="F36" s="22">
         <f t="shared" si="4"/>
         <v>1411</v>
       </c>
+      <c r="F36" s="21">
+        <f t="shared" si="5"/>
+        <v>1411</v>
+      </c>
     </row>
-    <row r="37" spans="2:6">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B37" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C37" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>521</v>
       </c>
       <c r="D37" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>547.04999999999995</v>
       </c>
       <c r="E37" s="7">
-        <f t="shared" si="3"/>
-        <v>521</v>
-      </c>
-      <c r="F37" s="22">
         <f t="shared" si="4"/>
         <v>521</v>
       </c>
+      <c r="F37" s="21">
+        <f t="shared" si="5"/>
+        <v>521</v>
+      </c>
     </row>
-    <row r="38" spans="2:6">
-      <c r="B38" s="29" t="s">
-        <v>32</v>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B38" s="28" t="s">
+        <v>31</v>
       </c>
       <c r="C38" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>568</v>
       </c>
       <c r="D38" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>612.15</v>
       </c>
       <c r="E38" s="7">
-        <f t="shared" si="3"/>
-        <v>583</v>
-      </c>
-      <c r="F38" s="22">
         <f t="shared" si="4"/>
         <v>583</v>
       </c>
+      <c r="F38" s="21">
+        <f t="shared" si="5"/>
+        <v>583</v>
+      </c>
     </row>
-    <row r="59" spans="2:6">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B39" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" s="7">
+        <f t="shared" si="2"/>
+        <v>568</v>
+      </c>
+      <c r="D39" s="7">
+        <f t="shared" ref="D39:D41" si="6">F39+(F39*5/100)</f>
+        <v>613.20000000000005</v>
+      </c>
+      <c r="E39" s="7">
+        <f t="shared" ref="E39:E41" si="7">F39</f>
+        <v>584</v>
+      </c>
+      <c r="F39" s="21">
+        <f t="shared" si="5"/>
+        <v>584</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B40" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40" s="7">
+        <f t="shared" si="2"/>
+        <v>568</v>
+      </c>
+      <c r="D40" s="7">
+        <f t="shared" si="6"/>
+        <v>614.25</v>
+      </c>
+      <c r="E40" s="7">
+        <f t="shared" si="7"/>
+        <v>585</v>
+      </c>
+      <c r="F40" s="21">
+        <f t="shared" si="5"/>
+        <v>585</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B41" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" s="7">
+        <f t="shared" si="2"/>
+        <v>568</v>
+      </c>
+      <c r="D41" s="7">
+        <f t="shared" si="6"/>
+        <v>615.29999999999995</v>
+      </c>
+      <c r="E41" s="7">
+        <f t="shared" si="7"/>
+        <v>586</v>
+      </c>
+      <c r="F41" s="21">
+        <f t="shared" si="5"/>
+        <v>586</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B59" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
       <c r="E59" s="1"/>
     </row>
-    <row r="60" spans="2:6">
-      <c r="B60" s="18" t="s">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B60" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C60" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E60" s="11"/>
+      <c r="F60" s="16"/>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B61" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C60" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E60" s="12"/>
-      <c r="F60" s="17"/>
+      <c r="C61" s="25">
+        <v>0</v>
+      </c>
+      <c r="D61" s="21">
+        <v>0</v>
+      </c>
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
     </row>
-    <row r="61" spans="2:6">
-      <c r="B61" s="6" t="s">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B62" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C61" s="26">
-        <v>0</v>
-      </c>
-      <c r="D61" s="22">
-        <v>0</v>
-      </c>
-      <c r="E61" s="13"/>
-      <c r="F61" s="13"/>
-    </row>
-    <row r="62" spans="2:6">
-      <c r="B62" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C62" s="28">
+      <c r="C62" s="27">
         <v>6.4999999999999997E-3</v>
       </c>
-      <c r="D62" s="27">
+      <c r="D62" s="26">
         <f>(F32-C32)/100</f>
         <v>0.65</v>
       </c>
-      <c r="E62" s="13"/>
-      <c r="F62" s="13"/>
+      <c r="E62" s="12"/>
+      <c r="F62" s="12"/>
     </row>
-    <row r="63" spans="2:6">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B63" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C63" s="28">
+        <v>26</v>
+      </c>
+      <c r="C63" s="27">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D63" s="27">
+      <c r="D63" s="26">
         <f>(F33-C33)/100</f>
         <v>0.4</v>
       </c>
-      <c r="E63" s="13"/>
-      <c r="F63" s="14"/>
+      <c r="E63" s="12"/>
+      <c r="F63" s="13"/>
     </row>
-    <row r="64" spans="2:6">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B64" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C64" s="27">
+        <v>-1.29E-2</v>
+      </c>
+      <c r="D64" s="26">
+        <f t="shared" ref="D64:D67" si="8">(F34-C34)/100</f>
+        <v>-1.29</v>
+      </c>
+      <c r="E64" s="12"/>
+      <c r="F64" s="13"/>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B65" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C64" s="28">
-        <v>-1.29E-2</v>
-      </c>
-      <c r="D64" s="27">
-        <f t="shared" ref="D64:D67" si="5">(F34-C34)/100</f>
-        <v>-1.29</v>
-      </c>
-      <c r="E64" s="13"/>
-      <c r="F64" s="14"/>
-    </row>
-    <row r="65" spans="2:6">
-      <c r="B65" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C65" s="28">
+      <c r="C65" s="27">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="D65" s="27">
+      <c r="D65" s="26">
         <f>(F35-C35)/100</f>
         <v>0.3</v>
       </c>
-      <c r="E65" s="14"/>
-      <c r="F65" s="14"/>
+      <c r="E65" s="13"/>
+      <c r="F65" s="13"/>
     </row>
-    <row r="66" spans="2:6">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B66" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C66" s="27">
+        <v>1.5E-3</v>
+      </c>
+      <c r="D66" s="26">
+        <f t="shared" si="8"/>
+        <v>0.15</v>
+      </c>
+      <c r="F66" s="13"/>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B67" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C66" s="28">
+      <c r="C67" s="27">
+        <v>0</v>
+      </c>
+      <c r="D67" s="26">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B68" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C68" s="27">
         <v>1.5E-3</v>
       </c>
-      <c r="D66" s="27">
-        <f t="shared" si="5"/>
-        <v>0.15</v>
-      </c>
-      <c r="F66" s="14"/>
-    </row>
-    <row r="67" spans="2:6">
-      <c r="B67" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C67" s="28">
-        <v>0</v>
-      </c>
-      <c r="D67" s="27">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="2:6">
-      <c r="B68" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="C68" s="28">
-        <v>1.5E-3</v>
-      </c>
-      <c r="D68" s="27">
+      <c r="D68" s="26">
         <f>(F38-C38)/100</f>
         <v>0.15</v>
       </c>
     </row>
-    <row r="69" spans="2:6">
-      <c r="C69" s="28"/>
-      <c r="D69" s="27"/>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B69" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C69" s="27">
+        <v>1.0015000000000001</v>
+      </c>
+      <c r="D69" s="26">
+        <f t="shared" ref="D69:D71" si="9">(F39-C39)/100</f>
+        <v>0.16</v>
+      </c>
     </row>
-    <row r="75" spans="2:6">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B70" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C70" s="27">
+        <v>2.0015000000000001</v>
+      </c>
+      <c r="D70" s="26">
+        <f t="shared" si="9"/>
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B71" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C71" s="27">
+        <v>3.0015000000000001</v>
+      </c>
+      <c r="D71" s="26">
+        <f t="shared" si="9"/>
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B75" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C75" s="5"/>
     </row>
-    <row r="76" spans="2:6">
-      <c r="B76" s="18" t="s">
+    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B76" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B77" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E76" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="77" spans="2:6">
-      <c r="B77" s="6" t="s">
-        <v>22</v>
       </c>
       <c r="C77" s="7">
         <v>0</v>
@@ -8687,11 +8989,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="2:6">
+    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B78" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C78" s="30">
+        <v>22</v>
+      </c>
+      <c r="C78" s="29">
         <f>E78-D78</f>
         <v>0</v>
       </c>
@@ -8704,16 +9006,16 @@
         <v>4482</v>
       </c>
     </row>
-    <row r="79" spans="2:6">
+    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B79" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C79" s="30">
-        <f t="shared" ref="C79:C84" si="6">E79-D79</f>
+        <v>26</v>
+      </c>
+      <c r="C79" s="29">
+        <f t="shared" ref="C79:C84" si="10">E79-D79</f>
         <v>200</v>
       </c>
       <c r="D79" s="7">
-        <f t="shared" ref="D79:D83" si="7">F33</f>
+        <f t="shared" ref="D79:D83" si="11">F33</f>
         <v>1007</v>
       </c>
       <c r="E79" s="7">
@@ -8721,16 +9023,16 @@
         <v>1207</v>
       </c>
     </row>
-    <row r="80" spans="2:6">
+    <row r="80" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B80" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C80" s="30">
-        <f t="shared" si="6"/>
+        <v>27</v>
+      </c>
+      <c r="C80" s="29">
+        <f t="shared" si="10"/>
         <v>300</v>
       </c>
       <c r="D80" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1197</v>
       </c>
       <c r="E80" s="7">
@@ -8738,16 +9040,16 @@
         <v>1497</v>
       </c>
     </row>
-    <row r="81" spans="2:5">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B81" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C81" s="30">
-        <f t="shared" si="6"/>
+        <v>28</v>
+      </c>
+      <c r="C81" s="29">
+        <f t="shared" si="10"/>
         <v>-35</v>
       </c>
       <c r="D81" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1441</v>
       </c>
       <c r="E81" s="7">
@@ -8755,16 +9057,16 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="82" spans="2:5">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B82" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C82" s="30">
-        <f t="shared" si="6"/>
+        <v>29</v>
+      </c>
+      <c r="C82" s="29">
+        <f t="shared" si="10"/>
         <v>50</v>
       </c>
       <c r="D82" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1411</v>
       </c>
       <c r="E82" s="7">
@@ -8772,16 +9074,16 @@
         <v>1461</v>
       </c>
     </row>
-    <row r="83" spans="2:5">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B83" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C83" s="30">
-        <f t="shared" si="6"/>
+        <v>30</v>
+      </c>
+      <c r="C83" s="29">
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="D83" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>521</v>
       </c>
       <c r="E83" s="7">
@@ -8789,12 +9091,12 @@
         <v>521</v>
       </c>
     </row>
-    <row r="84" spans="2:5">
-      <c r="B84" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="C84" s="30">
-        <f t="shared" si="6"/>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B84" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C84" s="29">
+        <f t="shared" si="10"/>
         <v>10</v>
       </c>
       <c r="D84" s="7">
@@ -8806,70 +9108,118 @@
         <v>593</v>
       </c>
     </row>
-    <row r="85" spans="2:5">
-      <c r="D85" s="7"/>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B85" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C85" s="29">
+        <f t="shared" ref="C85:C87" si="12">E85-D85</f>
+        <v>9</v>
+      </c>
+      <c r="D85" s="7">
+        <f t="shared" ref="D85:D87" si="13">F39</f>
+        <v>584</v>
+      </c>
+      <c r="E85" s="7">
+        <f t="shared" ref="E85:E87" si="14">583+10</f>
+        <v>593</v>
+      </c>
     </row>
-    <row r="92" spans="2:5">
-      <c r="B92" s="23"/>
-      <c r="C92" s="12"/>
-      <c r="D92" s="14"/>
-      <c r="E92" s="14"/>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B86" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C86" s="29">
+        <f t="shared" si="12"/>
+        <v>8</v>
+      </c>
+      <c r="D86" s="7">
+        <f t="shared" si="13"/>
+        <v>585</v>
+      </c>
+      <c r="E86" s="7">
+        <f t="shared" si="14"/>
+        <v>593</v>
+      </c>
     </row>
-    <row r="93" spans="2:5">
-      <c r="B93" s="12"/>
-      <c r="C93" s="12"/>
-      <c r="D93" s="12"/>
-      <c r="E93" s="12"/>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B87" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C87" s="29">
+        <f t="shared" si="12"/>
+        <v>7</v>
+      </c>
+      <c r="D87" s="7">
+        <f t="shared" si="13"/>
+        <v>586</v>
+      </c>
+      <c r="E87" s="7">
+        <f t="shared" si="14"/>
+        <v>593</v>
+      </c>
     </row>
-    <row r="94" spans="2:5">
-      <c r="B94" s="20"/>
-      <c r="C94" s="13"/>
-      <c r="D94" s="13"/>
-      <c r="E94" s="13"/>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B92" s="22"/>
+      <c r="C92" s="11"/>
+      <c r="D92" s="13"/>
+      <c r="E92" s="13"/>
     </row>
-    <row r="95" spans="2:5">
-      <c r="B95" s="20"/>
-      <c r="C95" s="13"/>
-      <c r="D95" s="13"/>
-      <c r="E95" s="13"/>
+    <row r="93" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B93" s="11"/>
+      <c r="C93" s="11"/>
+      <c r="D93" s="11"/>
+      <c r="E93" s="11"/>
     </row>
-    <row r="96" spans="2:5">
-      <c r="B96" s="20"/>
-      <c r="C96" s="13"/>
-      <c r="D96" s="24"/>
-      <c r="E96" s="13"/>
+    <row r="94" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B94" s="19"/>
+      <c r="C94" s="12"/>
+      <c r="D94" s="12"/>
+      <c r="E94" s="12"/>
     </row>
-    <row r="97" spans="2:5">
-      <c r="B97" s="20"/>
-      <c r="C97" s="13"/>
-      <c r="D97" s="24"/>
-      <c r="E97" s="13"/>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B95" s="19"/>
+      <c r="C95" s="12"/>
+      <c r="D95" s="12"/>
+      <c r="E95" s="12"/>
     </row>
-    <row r="102" spans="2:5">
+    <row r="96" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B96" s="19"/>
+      <c r="C96" s="12"/>
+      <c r="D96" s="23"/>
+      <c r="E96" s="12"/>
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B97" s="19"/>
+      <c r="C97" s="12"/>
+      <c r="D97" s="23"/>
+      <c r="E97" s="12"/>
+    </row>
+    <row r="102" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B102" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C102" s="5"/>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
     </row>
-    <row r="103" spans="2:5">
-      <c r="B103" s="18" t="s">
+    <row r="103" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B103" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E103" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B104" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D103" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E103" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="104" spans="2:5">
-      <c r="B104" s="6" t="s">
-        <v>22</v>
       </c>
       <c r="C104" s="7">
         <v>0</v>
@@ -8881,9 +9231,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="2:5">
+    <row r="105" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B105" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C105" s="7">
         <f>D105-E105</f>
@@ -8898,46 +9248,46 @@
         <v>4417</v>
       </c>
     </row>
-    <row r="106" spans="2:5">
+    <row r="106" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B106" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C106" s="7">
+        <f t="shared" ref="C106:C111" si="15">D106-E106</f>
+        <v>40</v>
+      </c>
+      <c r="D106" s="7">
+        <f t="shared" ref="D106:D110" si="16">F8</f>
+        <v>1007</v>
+      </c>
+      <c r="E106" s="7">
+        <f t="shared" ref="E106:E111" si="17">C8</f>
+        <v>967</v>
+      </c>
+    </row>
+    <row r="107" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B107" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C106" s="7">
-        <f t="shared" ref="C106:C111" si="8">D106-E106</f>
-        <v>40</v>
-      </c>
-      <c r="D106" s="7">
-        <f t="shared" ref="D106:D110" si="9">F8</f>
-        <v>1007</v>
-      </c>
-      <c r="E106" s="7">
-        <f t="shared" ref="E106:E111" si="10">C8</f>
-        <v>967</v>
+      <c r="C107" s="7">
+        <f t="shared" si="15"/>
+        <v>-129</v>
+      </c>
+      <c r="D107" s="7">
+        <f t="shared" si="16"/>
+        <v>1197</v>
+      </c>
+      <c r="E107" s="7">
+        <f t="shared" si="17"/>
+        <v>1326</v>
       </c>
     </row>
-    <row r="107" spans="2:5">
-      <c r="B107" s="8" t="s">
+    <row r="108" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B108" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C107" s="7">
-        <f t="shared" si="8"/>
-        <v>-129</v>
-      </c>
-      <c r="D107" s="7">
-        <f t="shared" si="9"/>
-        <v>1197</v>
-      </c>
-      <c r="E107" s="7">
-        <f t="shared" si="10"/>
-        <v>1326</v>
-      </c>
-    </row>
-    <row r="108" spans="2:5">
-      <c r="B108" s="8" t="s">
-        <v>29</v>
-      </c>
       <c r="C108" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>30</v>
       </c>
       <c r="D108" s="7">
@@ -8945,50 +9295,50 @@
         <v>1441</v>
       </c>
       <c r="E108" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>1411</v>
       </c>
     </row>
-    <row r="109" spans="2:5">
+    <row r="109" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B109" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C109" s="7">
+        <f t="shared" si="15"/>
+        <v>15</v>
+      </c>
+      <c r="D109" s="7">
+        <f t="shared" si="16"/>
+        <v>1411</v>
+      </c>
+      <c r="E109" s="7">
+        <f t="shared" si="17"/>
+        <v>1396</v>
+      </c>
+    </row>
+    <row r="110" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B110" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C109" s="7">
-        <f t="shared" si="8"/>
-        <v>15</v>
-      </c>
-      <c r="D109" s="7">
-        <f t="shared" si="9"/>
-        <v>1411</v>
-      </c>
-      <c r="E109" s="7">
-        <f t="shared" si="10"/>
-        <v>1396</v>
+      <c r="C110" s="7">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="D110" s="7">
+        <f t="shared" si="16"/>
+        <v>521</v>
+      </c>
+      <c r="E110" s="7">
+        <f t="shared" si="17"/>
+        <v>521</v>
       </c>
     </row>
-    <row r="110" spans="2:5">
-      <c r="B110" s="8" t="s">
+    <row r="111" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B111" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="C110" s="7">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="D110" s="7">
-        <f t="shared" si="9"/>
-        <v>521</v>
-      </c>
-      <c r="E110" s="7">
-        <f t="shared" si="10"/>
-        <v>521</v>
-      </c>
-    </row>
-    <row r="111" spans="2:5">
-      <c r="B111" s="29" t="s">
-        <v>32</v>
-      </c>
       <c r="C111" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>15</v>
       </c>
       <c r="D111" s="7">
@@ -8996,15 +9346,66 @@
         <v>583</v>
       </c>
       <c r="E111" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>568</v>
       </c>
     </row>
-    <row r="112" spans="2:5">
-      <c r="D112" s="7"/>
+    <row r="112" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B112" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C112" s="7">
+        <f t="shared" ref="C112:C114" si="18">D112-E112</f>
+        <v>16</v>
+      </c>
+      <c r="D112" s="7">
+        <f t="shared" ref="D112:D114" si="19">F14</f>
+        <v>584</v>
+      </c>
+      <c r="E112" s="7">
+        <f t="shared" ref="E112:E114" si="20">C14</f>
+        <v>568</v>
+      </c>
+    </row>
+    <row r="113" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B113" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C113" s="7">
+        <f t="shared" si="18"/>
+        <v>17</v>
+      </c>
+      <c r="D113" s="7">
+        <f t="shared" si="19"/>
+        <v>585</v>
+      </c>
+      <c r="E113" s="7">
+        <f t="shared" si="20"/>
+        <v>568</v>
+      </c>
+    </row>
+    <row r="114" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B114" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C114" s="7">
+        <f t="shared" si="18"/>
+        <v>18</v>
+      </c>
+      <c r="D114" s="7">
+        <f t="shared" si="19"/>
+        <v>586</v>
+      </c>
+      <c r="E114" s="7">
+        <f t="shared" si="20"/>
+        <v>568</v>
+      </c>
+    </row>
+    <row r="116" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D116" s="10"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -9015,11 +9416,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A007753-E669-4835-90BB-B57BBACA4DE7}">
   <dimension ref="C5:H21"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="G15" sqref="F15:G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="39.77734375" customWidth="1"/>
     <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
@@ -9029,21 +9430,21 @@
     <col min="8" max="8" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:8">
+    <row r="5" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="13"/>
+      <c r="G5" s="12"/>
     </row>
-    <row r="6" spans="3:8">
+    <row r="6" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C6" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>0</v>
@@ -9052,211 +9453,251 @@
         <v>1</v>
       </c>
       <c r="G6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="7" spans="3:8">
+    <row r="7" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="15">
+        <v>21</v>
+      </c>
+      <c r="D7" s="14">
         <f>G7/H7</f>
         <v>1</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="14">
         <v>0.6</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="14">
         <v>0.8</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="18">
         <v>3</v>
       </c>
-      <c r="H7" s="19">
+      <c r="H7" s="18">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="3:8">
+    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C8" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="15">
+        <v>22</v>
+      </c>
+      <c r="D8" s="14">
         <f>G8/H8</f>
         <v>1</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="14">
         <v>0.6</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="14">
         <v>0.8</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="18">
         <v>8</v>
       </c>
-      <c r="H8" s="19">
+      <c r="H8" s="18">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="3:8">
+    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C9" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="15">
+        <v>26</v>
+      </c>
+      <c r="D9" s="14">
         <f>G9/H9</f>
         <v>0.94444444444444442</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="14">
         <v>0.6</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="14">
         <v>0.8</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="18">
         <v>17</v>
       </c>
-      <c r="H9" s="19">
+      <c r="H9" s="18">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="3:8">
+    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C10" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="15">
+        <v>27</v>
+      </c>
+      <c r="D10" s="14">
         <f t="shared" ref="D10:D15" si="0">G10/H10</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="14">
         <v>0.6</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="14">
         <v>0.8</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="18">
         <v>12</v>
       </c>
-      <c r="H10" s="19">
+      <c r="H10" s="18">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="3:8">
+    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C11" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="15">
+        <v>28</v>
+      </c>
+      <c r="D11" s="14">
         <f t="shared" si="0"/>
         <v>0.77777777777777779</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="14">
         <v>0.6</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="14">
         <v>0.8</v>
       </c>
-      <c r="G11" s="31">
+      <c r="G11" s="30">
         <v>14</v>
       </c>
-      <c r="H11" s="19">
+      <c r="H11" s="18">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="3:8">
+    <row r="12" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C12" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="15">
+        <v>29</v>
+      </c>
+      <c r="D12" s="14">
         <f t="shared" si="0"/>
         <v>0.83333333333333337</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="14">
         <v>0.6</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="14">
         <v>0.8</v>
       </c>
-      <c r="G12" s="31">
+      <c r="G12" s="30">
         <v>15</v>
       </c>
-      <c r="H12" s="19">
+      <c r="H12" s="18">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="3:8">
+    <row r="13" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C13" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="15">
+        <v>30</v>
+      </c>
+      <c r="D13" s="14">
         <f t="shared" si="0"/>
         <v>0.83333333333333337</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="14">
         <v>0.6</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="14">
         <v>0.8</v>
       </c>
-      <c r="G13" s="31">
+      <c r="G13" s="30">
         <v>15</v>
       </c>
-      <c r="H13" s="19">
+      <c r="H13" s="18">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="3:8">
-      <c r="C14" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="15">
+    <row r="14" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C14" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="14">
         <f t="shared" si="0"/>
         <v>0.89473684210526316</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="14">
         <v>0.6</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="14">
         <v>0.8</v>
       </c>
-      <c r="G14" s="31">
+      <c r="G14" s="30">
         <v>17</v>
       </c>
-      <c r="H14" s="19">
+      <c r="H14" s="18">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="3:8">
-      <c r="C15" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="15">
-        <f t="shared" si="0"/>
-        <v>0.94736842105263153</v>
-      </c>
-      <c r="E15" s="15">
+    <row r="15" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C15" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="14">
+        <f t="shared" ref="D15:D17" si="1">G15/H15</f>
+        <v>0.89473684210526316</v>
+      </c>
+      <c r="E15" s="14">
         <v>0.6</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="14">
         <v>0.8</v>
       </c>
-      <c r="G15" s="31">
-        <v>18</v>
-      </c>
-      <c r="H15" s="19">
+      <c r="G15" s="30">
+        <v>17</v>
+      </c>
+      <c r="H15" s="18">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="6:6">
-      <c r="F17" s="11"/>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C16" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="14">
+        <f t="shared" si="1"/>
+        <v>0.89473684210526316</v>
+      </c>
+      <c r="E16" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="F16" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="G16" s="30">
+        <v>17</v>
+      </c>
+      <c r="H16" s="18">
+        <v>19</v>
+      </c>
     </row>
-    <row r="19" spans="6:6">
-      <c r="F19" s="11"/>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C17" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="14">
+        <f t="shared" si="1"/>
+        <v>0.89473684210526316</v>
+      </c>
+      <c r="E17" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="F17" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="G17" s="30">
+        <v>17</v>
+      </c>
+      <c r="H17" s="18">
+        <v>19</v>
+      </c>
     </row>
-    <row r="21" spans="6:6">
-      <c r="F21" s="11"/>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F19" s="10"/>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F21" s="10"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
inseriti dati dal pdp
</commit_message>
<xml_diff>
--- a/DocumentazioneEsterna/PianoDiQualifica/res/ResocontoAttivitaDiVerifica/res/metriche/grafici/qualitàProcesso/graficiProcessiOrganizzativi.xlsx
+++ b/DocumentazioneEsterna/PianoDiQualifica/res/ResocontoAttivitaDiVerifica/res/metriche/grafici/qualitàProcesso/graficiProcessiOrganizzativi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Università\Terzo anno\SWE\Progetto\Documentazione\DocumentazioneEsterna\PianoDiQualifica\res\ResocontoAttivitaDiVerifica\res\metriche\grafici\qualitàProcesso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FEE25AD-5A98-495A-8A00-53748BBC110B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520B6408-DF6B-4382-A8C1-306708AC73B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{32F62035-8081-4F2C-A1C6-0EA80AA4F9D3}"/>
   </bookViews>
@@ -618,13 +618,13 @@
                   <c:v>583</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>584</c:v>
+                  <c:v>947</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>585</c:v>
+                  <c:v>1090</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>586</c:v>
+                  <c:v>225</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -815,13 +815,13 @@
                   <c:v>568</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>568</c:v>
+                  <c:v>977</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>568</c:v>
+                  <c:v>1090</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>568</c:v>
+                  <c:v>225</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1325,13 +1325,13 @@
                   <c:v>612.15</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>613.20000000000005</c:v>
+                  <c:v>994.35</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>614.25</c:v>
+                  <c:v>1144.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>615.29999999999995</c:v>
+                  <c:v>236.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1440,13 +1440,13 @@
                   <c:v>583</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>584</c:v>
+                  <c:v>947</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>585</c:v>
+                  <c:v>1090</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>586</c:v>
+                  <c:v>225</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1661,13 +1661,13 @@
                   <c:v>568</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>568</c:v>
+                  <c:v>977</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>568</c:v>
+                  <c:v>1090</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>568</c:v>
+                  <c:v>225</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2280,13 +2280,13 @@
                   <c:v>1.5E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0015000000000001</c:v>
+                  <c:v>-3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.0015000000000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.0015000000000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2822,13 +2822,13 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3441,13 +3441,13 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16</c:v>
+                  <c:v>-30</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>17</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>18</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8289,8 +8289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EEB098D-590A-4332-807C-B47041EA10F7}">
   <dimension ref="B4:F116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="D116" sqref="D116"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="E112" sqref="E112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8443,7 +8443,7 @@
         <v>13154</v>
       </c>
       <c r="E12" s="7">
-        <f t="shared" si="0"/>
+        <f>F12</f>
         <v>521</v>
       </c>
       <c r="F12" s="7">
@@ -8461,7 +8461,7 @@
         <v>13154</v>
       </c>
       <c r="E13" s="7">
-        <f t="shared" si="0"/>
+        <f>F13</f>
         <v>583</v>
       </c>
       <c r="F13" s="7">
@@ -8473,17 +8473,17 @@
         <v>32</v>
       </c>
       <c r="C14" s="7">
-        <v>568</v>
+        <v>977</v>
       </c>
       <c r="D14" s="7">
         <v>13154</v>
       </c>
       <c r="E14" s="7">
         <f t="shared" ref="E14:E16" si="1">F14</f>
-        <v>584</v>
+        <v>947</v>
       </c>
       <c r="F14" s="7">
-        <v>584</v>
+        <v>947</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
@@ -8491,17 +8491,17 @@
         <v>33</v>
       </c>
       <c r="C15" s="7">
-        <v>568</v>
+        <v>1090</v>
       </c>
       <c r="D15" s="7">
         <v>13154</v>
       </c>
       <c r="E15" s="7">
         <f t="shared" si="1"/>
-        <v>585</v>
+        <v>1090</v>
       </c>
       <c r="F15" s="7">
-        <v>585</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
@@ -8509,17 +8509,17 @@
         <v>34</v>
       </c>
       <c r="C16" s="7">
-        <v>568</v>
+        <v>225</v>
       </c>
       <c r="D16" s="7">
         <v>13154</v>
       </c>
       <c r="E16" s="7">
         <f t="shared" si="1"/>
-        <v>586</v>
+        <v>225</v>
       </c>
       <c r="F16" s="7">
-        <v>586</v>
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
@@ -8735,19 +8735,19 @@
       </c>
       <c r="C39" s="7">
         <f t="shared" si="2"/>
-        <v>568</v>
+        <v>977</v>
       </c>
       <c r="D39" s="7">
         <f t="shared" ref="D39:D41" si="6">F39+(F39*5/100)</f>
-        <v>613.20000000000005</v>
+        <v>994.35</v>
       </c>
       <c r="E39" s="7">
         <f t="shared" ref="E39:E41" si="7">F39</f>
-        <v>584</v>
+        <v>947</v>
       </c>
       <c r="F39" s="21">
         <f t="shared" si="5"/>
-        <v>584</v>
+        <v>947</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.3">
@@ -8756,19 +8756,19 @@
       </c>
       <c r="C40" s="7">
         <f t="shared" si="2"/>
-        <v>568</v>
+        <v>1090</v>
       </c>
       <c r="D40" s="7">
         <f t="shared" si="6"/>
-        <v>614.25</v>
+        <v>1144.5</v>
       </c>
       <c r="E40" s="7">
         <f t="shared" si="7"/>
-        <v>585</v>
+        <v>1090</v>
       </c>
       <c r="F40" s="21">
         <f t="shared" si="5"/>
-        <v>585</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.3">
@@ -8777,19 +8777,19 @@
       </c>
       <c r="C41" s="7">
         <f t="shared" si="2"/>
-        <v>568</v>
+        <v>225</v>
       </c>
       <c r="D41" s="7">
         <f t="shared" si="6"/>
-        <v>615.29999999999995</v>
+        <v>236.25</v>
       </c>
       <c r="E41" s="7">
         <f t="shared" si="7"/>
-        <v>586</v>
+        <v>225</v>
       </c>
       <c r="F41" s="21">
         <f t="shared" si="5"/>
-        <v>586</v>
+        <v>225</v>
       </c>
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.3">
@@ -8924,11 +8924,11 @@
         <v>32</v>
       </c>
       <c r="C69" s="27">
-        <v>1.0015000000000001</v>
+        <v>-3.0000000000000001E-3</v>
       </c>
       <c r="D69" s="26">
         <f t="shared" ref="D69:D71" si="9">(F39-C39)/100</f>
-        <v>0.16</v>
+        <v>-0.3</v>
       </c>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.3">
@@ -8936,11 +8936,11 @@
         <v>33</v>
       </c>
       <c r="C70" s="27">
-        <v>2.0015000000000001</v>
+        <v>0</v>
       </c>
       <c r="D70" s="26">
         <f t="shared" si="9"/>
-        <v>0.17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.3">
@@ -8948,11 +8948,11 @@
         <v>34</v>
       </c>
       <c r="C71" s="27">
-        <v>3.0015000000000001</v>
+        <v>0</v>
       </c>
       <c r="D71" s="26">
         <f t="shared" si="9"/>
-        <v>0.18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="2:6" x14ac:dyDescent="0.3">
@@ -9114,15 +9114,15 @@
       </c>
       <c r="C85" s="29">
         <f t="shared" ref="C85:C87" si="12">E85-D85</f>
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="D85" s="7">
         <f t="shared" ref="D85:D87" si="13">F39</f>
-        <v>584</v>
+        <v>947</v>
       </c>
       <c r="E85" s="7">
-        <f t="shared" ref="E85:E87" si="14">583+10</f>
-        <v>593</v>
+        <f>947+28</f>
+        <v>975</v>
       </c>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.3">
@@ -9131,15 +9131,15 @@
       </c>
       <c r="C86" s="29">
         <f t="shared" si="12"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D86" s="7">
         <f t="shared" si="13"/>
-        <v>585</v>
+        <v>1090</v>
       </c>
       <c r="E86" s="7">
-        <f t="shared" si="14"/>
-        <v>593</v>
+        <f>1090+10</f>
+        <v>1100</v>
       </c>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.3">
@@ -9148,15 +9148,15 @@
       </c>
       <c r="C87" s="29">
         <f t="shared" si="12"/>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D87" s="7">
         <f t="shared" si="13"/>
-        <v>586</v>
+        <v>225</v>
       </c>
       <c r="E87" s="7">
-        <f t="shared" si="14"/>
-        <v>593</v>
+        <f>225</f>
+        <v>225</v>
       </c>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.3">
@@ -9253,15 +9253,15 @@
         <v>26</v>
       </c>
       <c r="C106" s="7">
-        <f t="shared" ref="C106:C111" si="15">D106-E106</f>
+        <f t="shared" ref="C106:C111" si="14">D106-E106</f>
         <v>40</v>
       </c>
       <c r="D106" s="7">
-        <f t="shared" ref="D106:D110" si="16">F8</f>
+        <f t="shared" ref="D106:D110" si="15">F8</f>
         <v>1007</v>
       </c>
       <c r="E106" s="7">
-        <f t="shared" ref="E106:E111" si="17">C8</f>
+        <f t="shared" ref="E106:E111" si="16">C8</f>
         <v>967</v>
       </c>
     </row>
@@ -9270,15 +9270,15 @@
         <v>27</v>
       </c>
       <c r="C107" s="7">
+        <f t="shared" si="14"/>
+        <v>-129</v>
+      </c>
+      <c r="D107" s="7">
         <f t="shared" si="15"/>
-        <v>-129</v>
-      </c>
-      <c r="D107" s="7">
+        <v>1197</v>
+      </c>
+      <c r="E107" s="7">
         <f t="shared" si="16"/>
-        <v>1197</v>
-      </c>
-      <c r="E107" s="7">
-        <f t="shared" si="17"/>
         <v>1326</v>
       </c>
     </row>
@@ -9287,7 +9287,7 @@
         <v>28</v>
       </c>
       <c r="C108" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>30</v>
       </c>
       <c r="D108" s="7">
@@ -9295,7 +9295,7 @@
         <v>1441</v>
       </c>
       <c r="E108" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>1411</v>
       </c>
     </row>
@@ -9304,15 +9304,15 @@
         <v>29</v>
       </c>
       <c r="C109" s="7">
+        <f t="shared" si="14"/>
+        <v>15</v>
+      </c>
+      <c r="D109" s="7">
         <f t="shared" si="15"/>
-        <v>15</v>
-      </c>
-      <c r="D109" s="7">
+        <v>1411</v>
+      </c>
+      <c r="E109" s="7">
         <f t="shared" si="16"/>
-        <v>1411</v>
-      </c>
-      <c r="E109" s="7">
-        <f t="shared" si="17"/>
         <v>1396</v>
       </c>
     </row>
@@ -9321,15 +9321,15 @@
         <v>30</v>
       </c>
       <c r="C110" s="7">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="D110" s="7">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="D110" s="7">
+        <v>521</v>
+      </c>
+      <c r="E110" s="7">
         <f t="shared" si="16"/>
-        <v>521</v>
-      </c>
-      <c r="E110" s="7">
-        <f t="shared" si="17"/>
         <v>521</v>
       </c>
     </row>
@@ -9338,7 +9338,7 @@
         <v>31</v>
       </c>
       <c r="C111" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>15</v>
       </c>
       <c r="D111" s="7">
@@ -9346,7 +9346,7 @@
         <v>583</v>
       </c>
       <c r="E111" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>568</v>
       </c>
     </row>
@@ -9355,16 +9355,16 @@
         <v>32</v>
       </c>
       <c r="C112" s="7">
-        <f t="shared" ref="C112:C114" si="18">D112-E112</f>
-        <v>16</v>
+        <f t="shared" ref="C112:C114" si="17">D112-E112</f>
+        <v>-30</v>
       </c>
       <c r="D112" s="7">
-        <f t="shared" ref="D112:D114" si="19">F14</f>
-        <v>584</v>
+        <f t="shared" ref="D112:D114" si="18">F14</f>
+        <v>947</v>
       </c>
       <c r="E112" s="7">
-        <f t="shared" ref="E112:E114" si="20">C14</f>
-        <v>568</v>
+        <f t="shared" ref="E112:E114" si="19">C14</f>
+        <v>977</v>
       </c>
     </row>
     <row r="113" spans="2:5" x14ac:dyDescent="0.3">
@@ -9372,16 +9372,16 @@
         <v>33</v>
       </c>
       <c r="C113" s="7">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="D113" s="7">
         <f t="shared" si="18"/>
-        <v>17</v>
-      </c>
-      <c r="D113" s="7">
+        <v>1090</v>
+      </c>
+      <c r="E113" s="7">
         <f t="shared" si="19"/>
-        <v>585</v>
-      </c>
-      <c r="E113" s="7">
-        <f t="shared" si="20"/>
-        <v>568</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="114" spans="2:5" x14ac:dyDescent="0.3">
@@ -9389,16 +9389,16 @@
         <v>34</v>
       </c>
       <c r="C114" s="7">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="D114" s="7">
         <f t="shared" si="18"/>
-        <v>18</v>
-      </c>
-      <c r="D114" s="7">
+        <v>225</v>
+      </c>
+      <c r="E114" s="7">
         <f t="shared" si="19"/>
-        <v>586</v>
-      </c>
-      <c r="E114" s="7">
-        <f t="shared" si="20"/>
-        <v>568</v>
+        <v>225</v>
       </c>
     </row>
     <row r="116" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Aggiornamento immagini per RA
</commit_message>
<xml_diff>
--- a/DocumentazioneEsterna/PianoDiQualifica/res/ResocontoAttivitaDiVerifica/res/metriche/grafici/qualitàProcesso/graficiProcessiOrganizzativi.xlsx
+++ b/DocumentazioneEsterna/PianoDiQualifica/res/ResocontoAttivitaDiVerifica/res/metriche/grafici/qualitàProcesso/graficiProcessiOrganizzativi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Università\Terzo anno\SWE\Progetto\Documentazione\DocumentazioneEsterna\PianoDiQualifica\res\ResocontoAttivitaDiVerifica\res\metriche\grafici\qualitàProcesso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520B6408-DF6B-4382-A8C1-306708AC73B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882B4460-BB1C-4383-975E-621CB061B551}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{32F62035-8081-4F2C-A1C6-0EA80AA4F9D3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{32F62035-8081-4F2C-A1C6-0EA80AA4F9D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Pianificazione" sheetId="1" r:id="rId1"/>
@@ -3939,31 +3939,40 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>GestioneQualità!$C$10:$C$17</c:f>
+              <c:f>GestioneQualità!$C$7:$C$17</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>PA</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Incremento 5</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Incremento 6</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>Incremento 7</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>Incremento 8</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>Incremento 9</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>Incremento 10</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>Incremento 11</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>Incremento 12</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>Incremento 13</c:v>
                 </c:pt>
               </c:strCache>
@@ -3971,32 +3980,41 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>GestioneQualità!$D$10:$D$17</c:f>
+              <c:f>GestioneQualità!$D$7:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.94444444444444442</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.66666666666666663</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>0.77777777777777779</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>0.83333333333333337</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>0.83333333333333337</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>0.89473684210526316</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>0.94736842105263153</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -4051,31 +4069,40 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>GestioneQualità!$C$10:$C$17</c:f>
+              <c:f>GestioneQualità!$C$7:$C$17</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>PA</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Incremento 5</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Incremento 6</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>Incremento 7</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>Incremento 8</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>Incremento 9</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>Incremento 10</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>Incremento 11</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>Incremento 12</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>Incremento 13</c:v>
                 </c:pt>
               </c:strCache>
@@ -4083,10 +4110,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>GestioneQualità!$E$10:$E$17</c:f>
+              <c:f>GestioneQualità!$E$7:$E$17</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.6</c:v>
                 </c:pt>
@@ -4109,6 +4136,15 @@
                   <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>0.6</c:v>
                 </c:pt>
               </c:numCache>
@@ -4149,31 +4185,40 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>GestioneQualità!$C$10:$C$17</c:f>
+              <c:f>GestioneQualità!$C$7:$C$17</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>PA</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Incremento 5</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Incremento 6</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>Incremento 7</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>Incremento 8</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>Incremento 9</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>Incremento 10</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>Incremento 11</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>Incremento 12</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>Incremento 13</c:v>
                 </c:pt>
               </c:strCache>
@@ -4181,10 +4226,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>GestioneQualità!$F$10:$F$17</c:f>
+              <c:f>GestioneQualità!$F$7:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.8</c:v>
                 </c:pt>
@@ -4207,6 +4252,15 @@
                   <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>0.8</c:v>
                 </c:pt>
               </c:numCache>
@@ -7951,16 +8005,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1371600</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1577340</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>564180</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>65520</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1280460</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>164580</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8289,7 +8343,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EEB098D-590A-4332-807C-B47041EA10F7}">
   <dimension ref="B4:F116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+    <sheetView topLeftCell="A166" workbookViewId="0">
       <selection activeCell="E112" sqref="E112"/>
     </sheetView>
   </sheetViews>
@@ -8425,7 +8479,7 @@
         <v>13154</v>
       </c>
       <c r="E11" s="7">
-        <f t="shared" ref="E11:E13" si="0">F11</f>
+        <f t="shared" ref="E11" si="0">F11</f>
         <v>1411</v>
       </c>
       <c r="F11" s="7">
@@ -9416,8 +9470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A007753-E669-4835-90BB-B57BBACA4DE7}">
   <dimension ref="C5:H21"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>